<commit_message>
Script de estacion y oficina
</commit_message>
<xml_diff>
--- a/scripts/Script.xlsx
+++ b/scripts/Script.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Lugar" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7774" uniqueCount="2355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7784" uniqueCount="2356">
   <si>
     <t>id</t>
   </si>
@@ -7095,6 +7095,9 @@
   </si>
   <si>
     <t>&lt;--Telefono jefe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -7448,7 +7451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
@@ -8407,7 +8410,7 @@
   <dimension ref="A1:X30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8418,6 +8421,7 @@
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="18" max="18" width="15.42578125" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" customWidth="1"/>
     <col min="22" max="22" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8471,23 +8475,26 @@
       <c r="T3" t="s">
         <v>63</v>
       </c>
+      <c r="U3" t="s">
+        <v>2355</v>
+      </c>
       <c r="V3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f t="shared" ref="A4:A30" si="0">CONCATENATE($A$2,G4)</f>
+        <f t="shared" ref="A4:A31" si="0">CONCATENATE($A$2,G4)</f>
         <v>Est. Dublin</v>
       </c>
       <c r="B4">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -8497,7 +8504,7 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" ref="I4:I30" si="1">CONCATENATE("('",A4,"', ",B4,", ",D4,", ",F4,"),")</f>
-        <v>('Est. Dublin', 28, 2, 10),</v>
+        <v>('Est. Dublin', 1, 11, 10),</v>
       </c>
       <c r="O4">
         <v>1</v>
@@ -8509,6 +8516,12 @@
       <c r="Q4">
         <v>0</v>
       </c>
+      <c r="R4">
+        <v>2</v>
+      </c>
+      <c r="T4" t="s">
+        <v>9</v>
+      </c>
       <c r="V4">
         <v>10</v>
       </c>
@@ -8516,8 +8529,8 @@
         <v>23</v>
       </c>
       <c r="X4" t="str">
-        <f t="shared" ref="X4" si="2">CONCATENATE("('",P4,"', '",Q4,"', ",R4,");")</f>
-        <v>('Ofi. Dublin', '0', );</v>
+        <f>CONCATENATE("('",P4,"', ",Q4,", ",R4,", ",T4,", ",V4,");")</f>
+        <v>('Ofi. Dublin', 0, 2, null, 10);</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -8532,7 +8545,8 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <f>D4+1</f>
+        <v>12</v>
       </c>
       <c r="F5">
         <v>11</v>
@@ -8542,7 +8556,7 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Cork', 1, 2, 11),</v>
+        <v>('Est. Cork', 1, 12, 11),</v>
       </c>
       <c r="O5">
         <f>O4+1</f>
@@ -8555,6 +8569,13 @@
       <c r="Q5">
         <v>0</v>
       </c>
+      <c r="R5">
+        <f t="shared" ref="R5:R12" si="2">R4+1</f>
+        <v>3</v>
+      </c>
+      <c r="T5" t="s">
+        <v>9</v>
+      </c>
       <c r="V5">
         <v>13</v>
       </c>
@@ -8562,8 +8583,8 @@
         <v>27</v>
       </c>
       <c r="X5" t="str">
-        <f>CONCATENATE("('",P5,"', '",Q5,"', ",R5,");")</f>
-        <v>('Ofi. Amsterdam', '0', );</v>
+        <f t="shared" ref="X5:X13" si="3">CONCATENATE("('",P5,"', ",Q5,", ",R5,", ",T5,", ",V5,");")</f>
+        <v>('Ofi. Amsterdam', 0, 3, null, 13);</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -8578,7 +8599,8 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <f t="shared" ref="D6:D30" si="4">D5+1</f>
+        <v>13</v>
       </c>
       <c r="F6">
         <v>12</v>
@@ -8588,10 +8610,10 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Galway', 1, 2, 12),</v>
+        <v>('Est. Galway', 1, 13, 12),</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6:O12" si="3">O5+1</f>
+        <f t="shared" ref="O6:O12" si="5">O5+1</f>
         <v>3</v>
       </c>
       <c r="P6" t="str">
@@ -8601,6 +8623,13 @@
       <c r="Q6">
         <v>0</v>
       </c>
+      <c r="R6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="T6" t="s">
+        <v>9</v>
+      </c>
       <c r="V6">
         <v>16</v>
       </c>
@@ -8608,8 +8637,8 @@
         <v>30</v>
       </c>
       <c r="X6" t="str">
-        <f>CONCATENATE("('",P6,"', '",Q6,"', ",R6,");")</f>
-        <v>('Ofi. Nuuk', '0', );</v>
+        <f t="shared" si="3"/>
+        <v>('Ofi. Nuuk', 0, 4, null, 16);</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -8618,13 +8647,15 @@
         <v>Est. Amsterdam</v>
       </c>
       <c r="B7">
-        <v>28</v>
+        <f>B4+1</f>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>14</v>
       </c>
       <c r="F7">
         <v>13</v>
@@ -8634,10 +8665,10 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Amsterdam', 28, 5, 13),</v>
+        <v>('Est. Amsterdam', 2, 14, 13),</v>
       </c>
       <c r="O7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="P7" t="str">
@@ -8647,6 +8678,13 @@
       <c r="Q7">
         <v>0</v>
       </c>
+      <c r="R7">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="T7" t="s">
+        <v>9</v>
+      </c>
       <c r="V7">
         <v>19</v>
       </c>
@@ -8654,8 +8692,8 @@
         <v>33</v>
       </c>
       <c r="X7" t="str">
-        <f>CONCATENATE("('",P7,"', '",Q7,"', ",R7,");")</f>
-        <v>('Ofi. Buenos Aires', '0', );</v>
+        <f t="shared" si="3"/>
+        <v>('Ofi. Buenos Aires', 0, 5, null, 19);</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -8664,14 +8702,15 @@
         <v>Est. Roterdam</v>
       </c>
       <c r="B8">
-        <f>B5+3</f>
-        <v>4</v>
+        <f>B5+1</f>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>15</v>
       </c>
       <c r="F8">
         <v>14</v>
@@ -8681,10 +8720,10 @@
       </c>
       <c r="I8" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Roterdam', 4, 5, 14),</v>
+        <v>('Est. Roterdam', 2, 15, 14),</v>
       </c>
       <c r="O8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="P8" t="str">
@@ -8694,6 +8733,13 @@
       <c r="Q8">
         <v>0</v>
       </c>
+      <c r="R8">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="T8" t="s">
+        <v>9</v>
+      </c>
       <c r="V8">
         <v>22</v>
       </c>
@@ -8701,8 +8747,8 @@
         <v>36</v>
       </c>
       <c r="X8" t="str">
-        <f>CONCATENATE("('",P8,"', '",Q8,"', ",R8,");")</f>
-        <v>('Ofi. Taipei', '0', );</v>
+        <f t="shared" si="3"/>
+        <v>('Ofi. Taipei', 0, 6, null, 22);</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -8711,14 +8757,15 @@
         <v>Est. Haarlam</v>
       </c>
       <c r="B9">
-        <f>B6+3</f>
-        <v>4</v>
+        <f>B6+1</f>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>16</v>
       </c>
       <c r="F9">
         <v>15</v>
@@ -8728,10 +8775,10 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Haarlam', 4, 5, 15),</v>
+        <v>('Est. Haarlam', 2, 16, 15),</v>
       </c>
       <c r="O9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="P9" t="str">
@@ -8741,7 +8788,14 @@
       <c r="Q9">
         <v>0</v>
       </c>
+      <c r="R9">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
       <c r="S9" s="1"/>
+      <c r="T9" t="s">
+        <v>9</v>
+      </c>
       <c r="V9">
         <v>25</v>
       </c>
@@ -8749,8 +8803,8 @@
         <v>39</v>
       </c>
       <c r="X9" t="str">
-        <f>CONCATENATE("('",P9,"', '",Q9,"', ",R9,");")</f>
-        <v>('Ofi. Kuala Lumpur', '0', );</v>
+        <f t="shared" si="3"/>
+        <v>('Ofi. Kuala Lumpur', 0, 7, null, 25);</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -8759,13 +8813,15 @@
         <v>Est. Nuuk</v>
       </c>
       <c r="B10">
-        <v>28</v>
+        <f t="shared" ref="B10:B30" si="6">B7+1</f>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <f t="shared" si="4"/>
+        <v>17</v>
       </c>
       <c r="F10">
         <v>16</v>
@@ -8775,10 +8831,10 @@
       </c>
       <c r="I10" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Nuuk', 28, 8, 16),</v>
+        <v>('Est. Nuuk', 3, 17, 16),</v>
       </c>
       <c r="O10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="P10" t="str">
@@ -8788,7 +8844,14 @@
       <c r="Q10">
         <v>0</v>
       </c>
+      <c r="R10">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
       <c r="S10" s="1"/>
+      <c r="T10" t="s">
+        <v>9</v>
+      </c>
       <c r="V10">
         <v>28</v>
       </c>
@@ -8796,8 +8859,8 @@
         <v>42</v>
       </c>
       <c r="X10" t="str">
-        <f>CONCATENATE("('",P10,"', '",Q10,"', ",R10,");")</f>
-        <v>('Ofi. Kampala', '0', );</v>
+        <f t="shared" si="3"/>
+        <v>('Ofi. Kampala', 0, 8, null, 28);</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -8806,14 +8869,15 @@
         <v>Est. Qaqortoq</v>
       </c>
       <c r="B11">
-        <f>B8+3</f>
-        <v>7</v>
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
       <c r="D11">
-        <v>8</v>
+        <f t="shared" si="4"/>
+        <v>18</v>
       </c>
       <c r="F11">
         <v>17</v>
@@ -8823,10 +8887,10 @@
       </c>
       <c r="I11" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Qaqortoq', 7, 8, 17),</v>
+        <v>('Est. Qaqortoq', 3, 18, 17),</v>
       </c>
       <c r="O11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="P11" t="str">
@@ -8836,7 +8900,14 @@
       <c r="Q11">
         <v>0</v>
       </c>
+      <c r="R11">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
       <c r="S11" s="1"/>
+      <c r="T11" t="s">
+        <v>9</v>
+      </c>
       <c r="V11">
         <v>31</v>
       </c>
@@ -8844,8 +8915,8 @@
         <v>45</v>
       </c>
       <c r="X11" t="str">
-        <f>CONCATENATE("('",P11,"', '",Q11,"', ",R11,");")</f>
-        <v>('Ofi. Harare', '0', );</v>
+        <f t="shared" si="3"/>
+        <v>('Ofi. Harare', 0, 9, null, 31);</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -8854,14 +8925,15 @@
         <v xml:space="preserve">Est. Sisimiut </v>
       </c>
       <c r="B12">
-        <f>B9+3</f>
-        <v>7</v>
+        <f t="shared" si="6"/>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <f t="shared" si="4"/>
+        <v>19</v>
       </c>
       <c r="F12">
         <v>18</v>
@@ -8871,10 +8943,10 @@
       </c>
       <c r="I12" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Sisimiut ', 7, 8, 18),</v>
+        <v>('Est. Sisimiut ', 3, 19, 18),</v>
       </c>
       <c r="O12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="P12" t="str">
@@ -8884,6 +8956,13 @@
       <c r="Q12">
         <v>0</v>
       </c>
+      <c r="R12">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="T12" t="s">
+        <v>9</v>
+      </c>
       <c r="V12">
         <v>34</v>
       </c>
@@ -8891,8 +8970,8 @@
         <v>48</v>
       </c>
       <c r="X12" t="str">
-        <f>CONCATENATE("('",P12,"', '",Q12,"', ",R12,");")</f>
-        <v>('Ofi. Sidney', '0', );</v>
+        <f t="shared" si="3"/>
+        <v>('Ofi. Sidney', 0, 10, null, 34);</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -8901,13 +8980,15 @@
         <v>Est. Buenos Aires</v>
       </c>
       <c r="B13">
-        <v>28</v>
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
       <c r="D13">
-        <v>11</v>
+        <f t="shared" si="4"/>
+        <v>20</v>
       </c>
       <c r="F13">
         <v>19</v>
@@ -8917,7 +8998,7 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Buenos Aires', 28, 11, 19),</v>
+        <v>('Est. Buenos Aires', 4, 20, 19),</v>
       </c>
       <c r="O13">
         <f>O12+1</f>
@@ -8930,18 +9011,21 @@
       <c r="Q13">
         <v>1</v>
       </c>
-      <c r="S13" t="s">
-        <v>52</v>
+      <c r="R13" t="s">
+        <v>9</v>
       </c>
       <c r="T13">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <v>38</v>
       </c>
       <c r="W13" t="s">
         <v>52</v>
       </c>
       <c r="X13" t="str">
-        <f>CONCATENATE("('",P13,"', '",Q13,"', ",R13,");")</f>
-        <v>('Ofi. Ginebra', '1', );</v>
+        <f t="shared" si="3"/>
+        <v>('Ofi. Ginebra', 1, null, 1, 38);</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -8950,14 +9034,15 @@
         <v>Est. Ciudad de Cordoba</v>
       </c>
       <c r="B14">
-        <f>B11+3</f>
-        <v>10</v>
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
       <c r="D14">
-        <v>11</v>
+        <f t="shared" si="4"/>
+        <v>21</v>
       </c>
       <c r="F14">
         <v>20</v>
@@ -8967,7 +9052,7 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Ciudad de Cordoba', 10, 11, 20),</v>
+        <v>('Est. Ciudad de Cordoba', 4, 21, 20),</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -8976,14 +9061,15 @@
         <v>Est. Rosario</v>
       </c>
       <c r="B15">
-        <f>B12+3</f>
-        <v>10</v>
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
       <c r="D15">
-        <v>11</v>
+        <f t="shared" si="4"/>
+        <v>22</v>
       </c>
       <c r="F15">
         <v>21</v>
@@ -8993,7 +9079,7 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Rosario', 10, 11, 21),</v>
+        <v>('Est. Rosario', 4, 22, 21),</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
@@ -9002,13 +9088,15 @@
         <v>Est. Taipei</v>
       </c>
       <c r="B16">
-        <v>28</v>
+        <f t="shared" si="6"/>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
       <c r="D16">
-        <v>14</v>
+        <f t="shared" si="4"/>
+        <v>23</v>
       </c>
       <c r="F16">
         <v>22</v>
@@ -9018,7 +9106,7 @@
       </c>
       <c r="I16" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Taipei', 28, 14, 22),</v>
+        <v>('Est. Taipei', 5, 23, 22),</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -9027,14 +9115,15 @@
         <v>Est. Tainan</v>
       </c>
       <c r="B17">
-        <f>B14+3</f>
-        <v>13</v>
+        <f t="shared" si="6"/>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
       </c>
       <c r="D17">
-        <v>14</v>
+        <f t="shared" si="4"/>
+        <v>24</v>
       </c>
       <c r="F17">
         <v>23</v>
@@ -9044,7 +9133,7 @@
       </c>
       <c r="I17" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Tainan', 13, 14, 23),</v>
+        <v>('Est. Tainan', 5, 24, 23),</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -9053,14 +9142,15 @@
         <v>Est. Kaohsiung</v>
       </c>
       <c r="B18">
-        <f>B15+3</f>
-        <v>13</v>
+        <f t="shared" si="6"/>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
         <v>15</v>
       </c>
       <c r="D18">
-        <v>14</v>
+        <f t="shared" si="4"/>
+        <v>25</v>
       </c>
       <c r="F18">
         <v>24</v>
@@ -9070,7 +9160,7 @@
       </c>
       <c r="I18" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Kaohsiung', 13, 14, 24),</v>
+        <v>('Est. Kaohsiung', 5, 25, 24),</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -9079,13 +9169,15 @@
         <v>Est. Kuala Lumpur</v>
       </c>
       <c r="B19">
-        <v>28</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
       </c>
       <c r="D19">
-        <v>17</v>
+        <f t="shared" si="4"/>
+        <v>26</v>
       </c>
       <c r="F19">
         <v>25</v>
@@ -9095,7 +9187,7 @@
       </c>
       <c r="I19" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Kuala Lumpur', 28, 17, 25),</v>
+        <v>('Est. Kuala Lumpur', 6, 26, 25),</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -9104,14 +9196,15 @@
         <v>Est. Malaca</v>
       </c>
       <c r="B20">
-        <f>B17+3</f>
-        <v>16</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
       </c>
       <c r="D20">
-        <v>17</v>
+        <f t="shared" si="4"/>
+        <v>27</v>
       </c>
       <c r="F20">
         <v>26</v>
@@ -9121,7 +9214,7 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Malaca', 16, 17, 26),</v>
+        <v>('Est. Malaca', 6, 27, 26),</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -9130,14 +9223,15 @@
         <v>Est. Pulau Pinang</v>
       </c>
       <c r="B21">
-        <f>B18+3</f>
-        <v>16</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
       </c>
       <c r="D21">
-        <v>17</v>
+        <f t="shared" si="4"/>
+        <v>28</v>
       </c>
       <c r="F21">
         <v>27</v>
@@ -9147,7 +9241,7 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Pulau Pinang', 16, 17, 27),</v>
+        <v>('Est. Pulau Pinang', 6, 28, 27),</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -9156,13 +9250,15 @@
         <v>Est. Kampala</v>
       </c>
       <c r="B22">
-        <v>28</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
       </c>
       <c r="D22">
-        <v>20</v>
+        <f t="shared" si="4"/>
+        <v>29</v>
       </c>
       <c r="F22">
         <v>28</v>
@@ -9172,7 +9268,7 @@
       </c>
       <c r="I22" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Kampala', 28, 20, 28),</v>
+        <v>('Est. Kampala', 7, 29, 28),</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -9181,14 +9277,15 @@
         <v>Est. Entebbe</v>
       </c>
       <c r="B23">
-        <f>B20+3</f>
-        <v>19</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
       </c>
       <c r="D23">
-        <v>20</v>
+        <f t="shared" si="4"/>
+        <v>30</v>
       </c>
       <c r="F23">
         <v>29</v>
@@ -9198,7 +9295,7 @@
       </c>
       <c r="I23" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Entebbe', 19, 20, 29),</v>
+        <v>('Est. Entebbe', 7, 30, 29),</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -9207,14 +9304,15 @@
         <v>Est. Kasese</v>
       </c>
       <c r="B24">
-        <f>B21+3</f>
-        <v>19</v>
+        <f t="shared" si="6"/>
+        <v>7</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
       </c>
       <c r="D24">
-        <v>20</v>
+        <f t="shared" si="4"/>
+        <v>31</v>
       </c>
       <c r="F24">
         <v>30</v>
@@ -9224,7 +9322,7 @@
       </c>
       <c r="I24" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Kasese', 19, 20, 30),</v>
+        <v>('Est. Kasese', 7, 31, 30),</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -9233,13 +9331,15 @@
         <v>Est. Harare</v>
       </c>
       <c r="B25">
-        <v>28</v>
+        <f t="shared" si="6"/>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
         <v>20</v>
       </c>
       <c r="D25">
-        <v>23</v>
+        <f t="shared" si="4"/>
+        <v>32</v>
       </c>
       <c r="F25">
         <v>31</v>
@@ -9249,7 +9349,7 @@
       </c>
       <c r="I25" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Harare', 28, 23, 31),</v>
+        <v>('Est. Harare', 8, 32, 31),</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -9258,14 +9358,15 @@
         <v>Est. Bulawayo</v>
       </c>
       <c r="B26">
-        <f>B23+3</f>
-        <v>22</v>
+        <f t="shared" si="6"/>
+        <v>8</v>
       </c>
       <c r="C26" t="s">
         <v>20</v>
       </c>
       <c r="D26">
-        <v>23</v>
+        <f t="shared" si="4"/>
+        <v>33</v>
       </c>
       <c r="F26">
         <v>32</v>
@@ -9275,7 +9376,7 @@
       </c>
       <c r="I26" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Bulawayo', 22, 23, 32),</v>
+        <v>('Est. Bulawayo', 8, 33, 32),</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -9284,14 +9385,15 @@
         <v>Est. Chitungwiza</v>
       </c>
       <c r="B27">
-        <f>B24+3</f>
-        <v>22</v>
+        <f t="shared" si="6"/>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
         <v>20</v>
       </c>
       <c r="D27">
-        <v>23</v>
+        <f t="shared" si="4"/>
+        <v>34</v>
       </c>
       <c r="F27">
         <v>33</v>
@@ -9301,7 +9403,7 @@
       </c>
       <c r="I27" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Chitungwiza', 22, 23, 33),</v>
+        <v>('Est. Chitungwiza', 8, 34, 33),</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -9310,13 +9412,15 @@
         <v>Est. Sidney</v>
       </c>
       <c r="B28">
-        <v>28</v>
+        <f t="shared" si="6"/>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
         <v>21</v>
       </c>
       <c r="D28">
-        <v>26</v>
+        <f t="shared" si="4"/>
+        <v>35</v>
       </c>
       <c r="F28">
         <v>34</v>
@@ -9326,7 +9430,7 @@
       </c>
       <c r="I28" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Sidney', 28, 26, 34),</v>
+        <v>('Est. Sidney', 9, 35, 34),</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -9335,14 +9439,15 @@
         <v>Est. Perth</v>
       </c>
       <c r="B29">
-        <f>B26+3</f>
-        <v>25</v>
+        <f t="shared" si="6"/>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
         <v>21</v>
       </c>
       <c r="D29">
-        <v>26</v>
+        <f t="shared" si="4"/>
+        <v>36</v>
       </c>
       <c r="F29">
         <v>35</v>
@@ -9352,7 +9457,7 @@
       </c>
       <c r="I29" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Perth', 25, 26, 35),</v>
+        <v>('Est. Perth', 9, 36, 35),</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -9361,14 +9466,15 @@
         <v>Est. Gold Coast</v>
       </c>
       <c r="B30">
-        <f>B27+3</f>
-        <v>25</v>
+        <f t="shared" si="6"/>
+        <v>9</v>
       </c>
       <c r="C30" t="s">
         <v>21</v>
       </c>
       <c r="D30">
-        <v>26</v>
+        <f t="shared" si="4"/>
+        <v>37</v>
       </c>
       <c r="F30">
         <v>36</v>
@@ -9378,7 +9484,7 @@
       </c>
       <c r="I30" t="str">
         <f t="shared" si="1"/>
-        <v>('Est. Gold Coast', 25, 26, 36),</v>
+        <v>('Est. Gold Coast', 9, 37, 36),</v>
       </c>
     </row>
   </sheetData>
@@ -30084,8 +30190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Script bien_empleado y oficina
</commit_message>
<xml_diff>
--- a/scripts/Script.xlsx
+++ b/scripts/Script.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Lugar" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7730" uniqueCount="2354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7741" uniqueCount="2356">
   <si>
     <t>id</t>
   </si>
@@ -7092,6 +7092,12 @@
   </si>
   <si>
     <t>INSERT INTO cuenta (año, presupuesto, fk_estacion, fk_oficina_principal) VALUES</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
@@ -8403,8 +8409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView topLeftCell="J2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8507,8 +8513,8 @@
         <f t="shared" ref="P4:P13" si="2">CONCATENATE($O$2,W4)</f>
         <v>Ofi. Dublin</v>
       </c>
-      <c r="Q4">
-        <v>0</v>
+      <c r="Q4" t="s">
+        <v>2355</v>
       </c>
       <c r="R4">
         <v>2</v>
@@ -8524,7 +8530,7 @@
       </c>
       <c r="X4" t="str">
         <f>CONCATENATE("('",P4,"', ",Q4,", ",R4,", ",T4,", ",V4,");")</f>
-        <v>('Ofi. Dublin', 0, 2, null, 10);</v>
+        <v>('Ofi. Dublin', false, 2, null, 10);</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -8560,8 +8566,8 @@
         <f t="shared" si="2"/>
         <v>Ofi. Amsterdam</v>
       </c>
-      <c r="Q5">
-        <v>0</v>
+      <c r="Q5" t="s">
+        <v>2355</v>
       </c>
       <c r="R5">
         <f t="shared" ref="R5:R12" si="3">R4+1</f>
@@ -8578,7 +8584,7 @@
       </c>
       <c r="X5" t="str">
         <f t="shared" ref="X5:X13" si="4">CONCATENATE("('",P5,"', ",Q5,", ",R5,", ",T5,", ",V5,");")</f>
-        <v>('Ofi. Amsterdam', 0, 3, null, 13);</v>
+        <v>('Ofi. Amsterdam', false, 3, null, 13);</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -8614,8 +8620,8 @@
         <f t="shared" si="2"/>
         <v>Ofi. Nuuk</v>
       </c>
-      <c r="Q6">
-        <v>0</v>
+      <c r="Q6" t="s">
+        <v>2355</v>
       </c>
       <c r="R6">
         <f t="shared" si="3"/>
@@ -8632,7 +8638,7 @@
       </c>
       <c r="X6" t="str">
         <f t="shared" si="4"/>
-        <v>('Ofi. Nuuk', 0, 4, null, 16);</v>
+        <v>('Ofi. Nuuk', false, 4, null, 16);</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -8669,8 +8675,8 @@
         <f t="shared" si="2"/>
         <v>Ofi. Buenos Aires</v>
       </c>
-      <c r="Q7">
-        <v>0</v>
+      <c r="Q7" t="s">
+        <v>2355</v>
       </c>
       <c r="R7">
         <f t="shared" si="3"/>
@@ -8687,7 +8693,7 @@
       </c>
       <c r="X7" t="str">
         <f t="shared" si="4"/>
-        <v>('Ofi. Buenos Aires', 0, 5, null, 19);</v>
+        <v>('Ofi. Buenos Aires', false, 5, null, 19);</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -8724,8 +8730,8 @@
         <f t="shared" si="2"/>
         <v>Ofi. Taipei</v>
       </c>
-      <c r="Q8">
-        <v>0</v>
+      <c r="Q8" t="s">
+        <v>2355</v>
       </c>
       <c r="R8">
         <f t="shared" si="3"/>
@@ -8742,7 +8748,7 @@
       </c>
       <c r="X8" t="str">
         <f t="shared" si="4"/>
-        <v>('Ofi. Taipei', 0, 6, null, 22);</v>
+        <v>('Ofi. Taipei', false, 6, null, 22);</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -8779,8 +8785,8 @@
         <f t="shared" si="2"/>
         <v>Ofi. Kuala Lumpur</v>
       </c>
-      <c r="Q9">
-        <v>0</v>
+      <c r="Q9" t="s">
+        <v>2355</v>
       </c>
       <c r="R9">
         <f t="shared" si="3"/>
@@ -8798,7 +8804,7 @@
       </c>
       <c r="X9" t="str">
         <f t="shared" si="4"/>
-        <v>('Ofi. Kuala Lumpur', 0, 7, null, 25);</v>
+        <v>('Ofi. Kuala Lumpur', false, 7, null, 25);</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -8835,8 +8841,8 @@
         <f t="shared" si="2"/>
         <v>Ofi. Kampala</v>
       </c>
-      <c r="Q10">
-        <v>0</v>
+      <c r="Q10" t="s">
+        <v>2355</v>
       </c>
       <c r="R10">
         <f t="shared" si="3"/>
@@ -8854,7 +8860,7 @@
       </c>
       <c r="X10" t="str">
         <f t="shared" si="4"/>
-        <v>('Ofi. Kampala', 0, 8, null, 28);</v>
+        <v>('Ofi. Kampala', false, 8, null, 28);</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
@@ -8891,8 +8897,8 @@
         <f t="shared" si="2"/>
         <v>Ofi. Harare</v>
       </c>
-      <c r="Q11">
-        <v>0</v>
+      <c r="Q11" t="s">
+        <v>2355</v>
       </c>
       <c r="R11">
         <f t="shared" si="3"/>
@@ -8910,7 +8916,7 @@
       </c>
       <c r="X11" t="str">
         <f t="shared" si="4"/>
-        <v>('Ofi. Harare', 0, 9, null, 31);</v>
+        <v>('Ofi. Harare', false, 9, null, 31);</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -8947,8 +8953,8 @@
         <f t="shared" si="2"/>
         <v>Ofi. Sidney</v>
       </c>
-      <c r="Q12">
-        <v>0</v>
+      <c r="Q12" t="s">
+        <v>2355</v>
       </c>
       <c r="R12">
         <f t="shared" si="3"/>
@@ -8965,7 +8971,7 @@
       </c>
       <c r="X12" t="str">
         <f t="shared" si="4"/>
-        <v>('Ofi. Sidney', 0, 10, null, 34);</v>
+        <v>('Ofi. Sidney', false, 10, null, 34);</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -9002,8 +9008,8 @@
         <f t="shared" si="2"/>
         <v>Ofi. Ginebra</v>
       </c>
-      <c r="Q13">
-        <v>1</v>
+      <c r="Q13" t="s">
+        <v>2354</v>
       </c>
       <c r="R13" t="s">
         <v>9</v>
@@ -9019,7 +9025,7 @@
       </c>
       <c r="X13" t="str">
         <f t="shared" si="4"/>
-        <v>('Ofi. Ginebra', 1, null, 1, 38);</v>
+        <v>('Ofi. Ginebra', true, null, 1, 38);</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -30184,8 +30190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30264,9 +30270,12 @@
       <c r="H4">
         <v>412.23900209999999</v>
       </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
       <c r="K4" t="str">
-        <f>CONCATENATE("(",B4,", ", C4,", ", D4,", ", E4, ", ", F4,", ",G4,"),")</f>
-        <v>('Brandon', 'Constantino', 'Razo', 'Casillas', ROW(412,2390021), director_ejecutivo),</v>
+        <f>CONCATENATE("(",B4,", ", C4,", ", D4,", ", E4, ", ", F4,", ",G4,", ",I4,"),")</f>
+        <v>('Brandon', 'Constantino', 'Razo', 'Casillas', ROW(412,2390021), director_ejecutivo, null),</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -30300,8 +30309,8 @@
         <v>1</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" ref="K5:K31" si="1">CONCATENATE("(",B5,", ", C5,", ", D5,", ", E5, ", ", F5,", ",G5,"),")</f>
-        <v>('Elian', 'Maximo', 'Carter', 'Silva', ROW(412,6699623), director_area),</v>
+        <f t="shared" ref="K5:K40" si="1">CONCATENATE("(",B5,", ", C5,", ", D5,", ", E5, ", ", F5,", ",G5,", ",I5,"),")</f>
+        <v>('Elian', 'Maximo', 'Carter', 'Silva', ROW(412,6699623), director_area, 1),</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -30336,7 +30345,7 @@
       </c>
       <c r="K6" t="str">
         <f t="shared" si="1"/>
-        <v>('Fabiano', 'Tarsicio', 'Santamaria', 'Jaquez', ROW(412,3948307), director_area),</v>
+        <v>('Fabiano', 'Tarsicio', 'Santamaria', 'Jaquez', ROW(412,3948307), director_area, 1),</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -30371,7 +30380,7 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="1"/>
-        <v>('Esperanza', 'Ana', 'Corona', 'Granados', ROW(412,1189159), director_area),</v>
+        <v>('Esperanza', 'Ana', 'Corona', 'Granados', ROW(412,1189159), director_area, 1),</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -30406,7 +30415,7 @@
       </c>
       <c r="K8" t="str">
         <f t="shared" si="1"/>
-        <v>('Octavia', 'Eduviges', 'Mena', 'Alcantara', ROW(412,3974651), director_area),</v>
+        <v>('Octavia', 'Eduviges', 'Mena', 'Alcantara', ROW(412,3974651), director_area, 1),</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -30441,7 +30450,7 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
-        <v>('Anthony', 'Amilcar', 'Tafoya', 'Buenrostro', ROW(414,1319978), director_area),</v>
+        <v>('Anthony', 'Amilcar', 'Tafoya', 'Buenrostro', ROW(414,1319978), director_area, 1),</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -30476,7 +30485,7 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v>('Fidel', 'Juan', 'Regalado', 'Machuca', ROW(416,7319514), director_area),</v>
+        <v>('Fidel', 'Juan', 'Regalado', 'Machuca', ROW(416,7319514), director_area, 1),</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -30511,7 +30520,7 @@
       </c>
       <c r="K11" t="str">
         <f t="shared" si="1"/>
-        <v>('Luna', 'Judith', 'Castrejon', 'Narvaez', ROW(412,6345573), director_area),</v>
+        <v>('Luna', 'Judith', 'Castrejon', 'Narvaez', ROW(412,6345573), director_area, 1),</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -30546,7 +30555,7 @@
       </c>
       <c r="K12" t="str">
         <f t="shared" si="1"/>
-        <v>('Klement', 'Klement', 'Montiel', 'Salguero', ROW(414,3977631), director_area),</v>
+        <v>('Klement', 'Klement', 'Montiel', 'Salguero', ROW(414,3977631), director_area, 1),</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -30581,7 +30590,7 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="1"/>
-        <v>('Daniel', 'Italo', 'Price', 'Gallardo', ROW(414,3609837), director_area),</v>
+        <v>('Daniel', 'Italo', 'Price', 'Gallardo', ROW(414,3609837), director_area, 1),</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -30616,7 +30625,7 @@
       </c>
       <c r="K14" t="str">
         <f t="shared" si="1"/>
-        <v>('Silvester', 'Vitalicio', 'Morris', 'Serrato', ROW(412,5343364), jefe),</v>
+        <v>('Silvester', 'Vitalicio', 'Morris', 'Serrato', ROW(412,5343364), jefe, 2),</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -30651,7 +30660,7 @@
       </c>
       <c r="K15" t="str">
         <f t="shared" si="1"/>
-        <v>('Pamela', 'Irma', 'Guevara', 'Zapata', ROW(424,2908908), jefe),</v>
+        <v>('Pamela', 'Irma', 'Guevara', 'Zapata', ROW(424,2908908), jefe, 2),</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -30686,7 +30695,7 @@
       </c>
       <c r="K16" t="str">
         <f t="shared" si="1"/>
-        <v>('Feliciano', 'Jaime', 'Hurtado', 'Baca', ROW(424,2109538), jefe),</v>
+        <v>('Feliciano', 'Jaime', 'Hurtado', 'Baca', ROW(424,2109538), jefe, 2),</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -30721,7 +30730,7 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" si="1"/>
-        <v>('Eloisa', 'Petronila', 'Nolasco', 'White', ROW(414,6830298), jefe),</v>
+        <v>('Eloisa', 'Petronila', 'Nolasco', 'White', ROW(414,6830298), jefe, 3),</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -30756,7 +30765,7 @@
       </c>
       <c r="K18" t="str">
         <f t="shared" si="1"/>
-        <v>('Cayetano', 'Paulo', 'Guillen', 'Miramontes', ROW(412,4866865), jefe),</v>
+        <v>('Cayetano', 'Paulo', 'Guillen', 'Miramontes', ROW(412,4866865), jefe, 3),</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -30791,7 +30800,7 @@
       </c>
       <c r="K19" t="str">
         <f t="shared" si="1"/>
-        <v>('Constantino', 'Adolfo', 'Bustos', 'Lima', ROW(412,2392031), jefe),</v>
+        <v>('Constantino', 'Adolfo', 'Bustos', 'Lima', ROW(412,2392031), jefe, 3),</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -30826,7 +30835,7 @@
       </c>
       <c r="K20" t="str">
         <f t="shared" si="1"/>
-        <v>('Antonio', 'Tulio', 'Pinto', 'Cordero', ROW(416,3952857), jefe),</v>
+        <v>('Antonio', 'Tulio', 'Pinto', 'Cordero', ROW(416,3952857), jefe, 4),</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -30861,7 +30870,7 @@
       </c>
       <c r="K21" t="str">
         <f t="shared" si="1"/>
-        <v>('Dulcinea', 'Consuelo', 'Pizarro', 'Santiago', ROW(416,7676921), jefe),</v>
+        <v>('Dulcinea', 'Consuelo', 'Pizarro', 'Santiago', ROW(416,7676921), jefe, 4),</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -30896,7 +30905,7 @@
       </c>
       <c r="K22" t="str">
         <f t="shared" si="1"/>
-        <v>('Marsello', 'Alan', 'Carpio', 'Thomas', ROW(414,7291221), jefe),</v>
+        <v>('Marsello', 'Alan', 'Carpio', 'Thomas', ROW(414,7291221), jefe, 4),</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -30931,7 +30940,7 @@
       </c>
       <c r="K23" t="str">
         <f t="shared" si="1"/>
-        <v>('Antonio', 'Diego', 'Recinos', 'Santacruz', ROW(414,4392478), jefe),</v>
+        <v>('Antonio', 'Diego', 'Recinos', 'Santacruz', ROW(414,4392478), jefe, 5),</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -30966,7 +30975,7 @@
       </c>
       <c r="K24" t="str">
         <f t="shared" si="1"/>
-        <v>('Greta', 'Rosaura', 'Valdivia', 'Cruz', ROW(416,1080469), jefe),</v>
+        <v>('Greta', 'Rosaura', 'Valdivia', 'Cruz', ROW(416,1080469), jefe, 5),</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -31001,7 +31010,7 @@
       </c>
       <c r="K25" t="str">
         <f t="shared" si="1"/>
-        <v>('Marcela', 'Amelia', 'Galdamez', 'Rogers', ROW(412,6909353), jefe),</v>
+        <v>('Marcela', 'Amelia', 'Galdamez', 'Rogers', ROW(412,6909353), jefe, 5),</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -31036,7 +31045,7 @@
       </c>
       <c r="K26" t="str">
         <f t="shared" si="1"/>
-        <v>('Pamela', 'Veronica', 'Torres', 'Diaz', ROW(414,1416359), jefe),</v>
+        <v>('Pamela', 'Veronica', 'Torres', 'Diaz', ROW(414,1416359), jefe, 6),</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -31071,7 +31080,7 @@
       </c>
       <c r="K27" t="str">
         <f t="shared" si="1"/>
-        <v>('Cayetano', 'Fulgencio', 'Marquez', 'Infante', ROW(424,9630352), jefe),</v>
+        <v>('Cayetano', 'Fulgencio', 'Marquez', 'Infante', ROW(424,9630352), jefe, 6),</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -31106,7 +31115,7 @@
       </c>
       <c r="K28" t="str">
         <f t="shared" si="1"/>
-        <v>('Jhoan', 'Dante', 'Lucero', 'Orona', ROW(424,6170815), jefe),</v>
+        <v>('Jhoan', 'Dante', 'Lucero', 'Orona', ROW(424,6170815), jefe, 6),</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -31141,7 +31150,7 @@
       </c>
       <c r="K29" t="str">
         <f t="shared" si="1"/>
-        <v>('Elidio', 'Jonathan', 'Puentes', 'Ozuna', ROW(416,7058298), jefe),</v>
+        <v>('Elidio', 'Jonathan', 'Puentes', 'Ozuna', ROW(416,7058298), jefe, 7),</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -31176,7 +31185,7 @@
       </c>
       <c r="K30" t="str">
         <f t="shared" si="1"/>
-        <v>('Gloria', 'Eneida', 'Duque', 'Uribe', ROW(412,4224557), jefe),</v>
+        <v>('Gloria', 'Eneida', 'Duque', 'Uribe', ROW(412,4224557), jefe, 7),</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -31211,7 +31220,7 @@
       </c>
       <c r="K31" t="str">
         <f t="shared" si="1"/>
-        <v>('Jennifer', 'Valentina', 'Vigil', 'Aviles', ROW(424,9270841), jefe),</v>
+        <v>('Jennifer', 'Valentina', 'Vigil', 'Aviles', ROW(424,9270841), jefe, 7),</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -31245,8 +31254,8 @@
         <v>8</v>
       </c>
       <c r="K32" t="str">
-        <f t="shared" ref="K32:K40" si="4">CONCATENATE("(",B32,", ", C32,", ", D32,", ", E32, ", ", F32,", ",G32,"),")</f>
-        <v>('Celeste', 'Soledad', 'Chacon', 'Machado', ROW(412,1229016), jefe),</v>
+        <f t="shared" si="1"/>
+        <v>('Celeste', 'Soledad', 'Chacon', 'Machado', ROW(412,1229016), jefe, 8),</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -31280,8 +31289,8 @@
         <v>8</v>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="4"/>
-        <v>('Vivaldo', 'Tarsicio', 'Rosas', 'Jackson', ROW(412,5018092), jefe),</v>
+        <f t="shared" si="1"/>
+        <v>('Vivaldo', 'Tarsicio', 'Rosas', 'Jackson', ROW(412,5018092), jefe, 8),</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -31315,8 +31324,8 @@
         <v>8</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="4"/>
-        <v>('Mirella', 'Zamira', 'Machuca', 'Magallon', ROW(416,3371835), jefe),</v>
+        <f t="shared" si="1"/>
+        <v>('Mirella', 'Zamira', 'Machuca', 'Magallon', ROW(416,3371835), jefe, 8),</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -31350,8 +31359,8 @@
         <v>9</v>
       </c>
       <c r="K35" t="str">
-        <f t="shared" si="4"/>
-        <v>('Calixtrato', 'Vicente', 'Quintanilla', 'Estrada', ROW(414,3049959), jefe),</v>
+        <f t="shared" si="1"/>
+        <v>('Calixtrato', 'Vicente', 'Quintanilla', 'Estrada', ROW(414,3049959), jefe, 9),</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -31385,8 +31394,8 @@
         <v>9</v>
       </c>
       <c r="K36" t="str">
-        <f t="shared" si="4"/>
-        <v>('Libertad', 'Eliana', 'Garces', 'Casanova', ROW(414,8123924), jefe),</v>
+        <f t="shared" si="1"/>
+        <v>('Libertad', 'Eliana', 'Garces', 'Casanova', ROW(414,8123924), jefe, 9),</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -31420,8 +31429,8 @@
         <v>9</v>
       </c>
       <c r="K37" t="str">
-        <f t="shared" si="4"/>
-        <v>('Emperatriz', 'Myriam', 'Angulo', 'Valdivia', ROW(4148,999846), jefe),</v>
+        <f t="shared" si="1"/>
+        <v>('Emperatriz', 'Myriam', 'Angulo', 'Valdivia', ROW(4148,999846), jefe, 9),</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -31455,8 +31464,8 @@
         <v>10</v>
       </c>
       <c r="K38" t="str">
-        <f t="shared" si="4"/>
-        <v>('Hugo', 'Adan', 'Serrato', 'Barrios', ROW(416,1450123), jefe),</v>
+        <f t="shared" si="1"/>
+        <v>('Hugo', 'Adan', 'Serrato', 'Barrios', ROW(416,1450123), jefe, 10),</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -31490,8 +31499,8 @@
         <v>10</v>
       </c>
       <c r="K39" t="str">
-        <f t="shared" si="4"/>
-        <v>('Rosalia', 'Pilar', 'Valles', 'Montes', ROW(414,1292334), jefe),</v>
+        <f t="shared" si="1"/>
+        <v>('Rosalia', 'Pilar', 'Valles', 'Montes', ROW(414,1292334), jefe, 10),</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -31525,8 +31534,8 @@
         <v>10</v>
       </c>
       <c r="K40" t="str">
-        <f t="shared" si="4"/>
-        <v>('Claudio', 'Lincoln', 'Sullivan', 'Tafoya', ROW(412,1948734), jefe),</v>
+        <f t="shared" si="1"/>
+        <v>('Claudio', 'Lincoln', 'Sullivan', 'Tafoya', ROW(412,1948734), jefe, 10),</v>
       </c>
     </row>
   </sheetData>
@@ -41595,7 +41604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
@@ -41878,7 +41887,7 @@
         <v>27</v>
       </c>
       <c r="F13">
-        <f>F4+1</f>
+        <f t="shared" ref="F13:F21" si="2">F4+1</f>
         <v>2</v>
       </c>
       <c r="H13" t="str">
@@ -41907,7 +41916,7 @@
         <v>27</v>
       </c>
       <c r="F14">
-        <f>F5+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H14" t="str">
@@ -41936,7 +41945,7 @@
         <v>27</v>
       </c>
       <c r="F15">
-        <f>F6+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H15" t="str">
@@ -41965,7 +41974,7 @@
         <v>28</v>
       </c>
       <c r="F16">
-        <f>F7+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H16" t="str">
@@ -41994,7 +42003,7 @@
         <v>28</v>
       </c>
       <c r="F17">
-        <f>F8+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H17" t="str">
@@ -42023,7 +42032,7 @@
         <v>28</v>
       </c>
       <c r="F18">
-        <f>F9+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H18" t="str">
@@ -42052,7 +42061,7 @@
         <v>29</v>
       </c>
       <c r="F19">
-        <f>F10+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H19" t="str">
@@ -42081,7 +42090,7 @@
         <v>29</v>
       </c>
       <c r="F20">
-        <f>F11+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H20" t="str">
@@ -42110,7 +42119,7 @@
         <v>29</v>
       </c>
       <c r="F21">
-        <f>F12+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H21" t="str">
@@ -42139,7 +42148,7 @@
         <v>30</v>
       </c>
       <c r="F22">
-        <f t="shared" ref="F22:F85" si="2">F13+1</f>
+        <f t="shared" ref="F22:F84" si="3">F13+1</f>
         <v>3</v>
       </c>
       <c r="H22" t="str">
@@ -42168,7 +42177,7 @@
         <v>30</v>
       </c>
       <c r="F23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="H23" t="str">
@@ -42197,7 +42206,7 @@
         <v>30</v>
       </c>
       <c r="F24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="H24" t="str">
@@ -42226,7 +42235,7 @@
         <v>31</v>
       </c>
       <c r="F25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="H25" t="str">
@@ -42255,7 +42264,7 @@
         <v>31</v>
       </c>
       <c r="F26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="H26" t="str">
@@ -42284,7 +42293,7 @@
         <v>31</v>
       </c>
       <c r="F27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="H27" t="str">
@@ -42313,7 +42322,7 @@
         <v>32</v>
       </c>
       <c r="F28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="H28" t="str">
@@ -42342,7 +42351,7 @@
         <v>32</v>
       </c>
       <c r="F29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="H29" t="str">
@@ -42371,7 +42380,7 @@
         <v>32</v>
       </c>
       <c r="F30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="H30" t="str">
@@ -42400,7 +42409,7 @@
         <v>33</v>
       </c>
       <c r="F31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="H31" t="str">
@@ -42429,7 +42438,7 @@
         <v>33</v>
       </c>
       <c r="F32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="H32" t="str">
@@ -42458,7 +42467,7 @@
         <v>33</v>
       </c>
       <c r="F33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="H33" t="str">
@@ -42481,7 +42490,7 @@
         <v>34</v>
       </c>
       <c r="F34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="H34" t="str">
@@ -42504,7 +42513,7 @@
         <v>34</v>
       </c>
       <c r="F35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="H35" t="str">
@@ -42527,11 +42536,11 @@
         <v>34</v>
       </c>
       <c r="F36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" ref="H36:H67" si="3">CONCATENATE("('", A36,"',  ",B36,", ",C36,", ",F36,"),")</f>
+        <f t="shared" ref="H36:H67" si="4">CONCATENATE("('", A36,"',  ",B36,", ",C36,", ",F36,"),")</f>
         <v>('2036/31/12',  11500, 11, 4),</v>
       </c>
     </row>
@@ -42550,11 +42559,11 @@
         <v>35</v>
       </c>
       <c r="F37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2034/31/12',  10000, 12, 4),</v>
       </c>
     </row>
@@ -42573,11 +42582,11 @@
         <v>35</v>
       </c>
       <c r="F38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2035/31/12',  10500, 12, 4),</v>
       </c>
     </row>
@@ -42596,11 +42605,11 @@
         <v>35</v>
       </c>
       <c r="F39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2036/31/12',  11000, 12, 4),</v>
       </c>
     </row>
@@ -42619,11 +42628,11 @@
         <v>36</v>
       </c>
       <c r="F40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2034/31/12',  10000, 13, 5),</v>
       </c>
     </row>
@@ -42642,11 +42651,11 @@
         <v>36</v>
       </c>
       <c r="F41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2035/31/12',  10500, 13, 5),</v>
       </c>
     </row>
@@ -42665,11 +42674,11 @@
         <v>36</v>
       </c>
       <c r="F42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="H42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2036/31/12',  11000, 13, 5),</v>
       </c>
     </row>
@@ -42688,11 +42697,11 @@
         <v>37</v>
       </c>
       <c r="F43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="H43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2034/31/12',  12000, 14, 5),</v>
       </c>
     </row>
@@ -42711,11 +42720,11 @@
         <v>37</v>
       </c>
       <c r="F44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="H44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2035/31/12',  13000, 14, 5),</v>
       </c>
     </row>
@@ -42734,11 +42743,11 @@
         <v>37</v>
       </c>
       <c r="F45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="H45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2036/31/12',  10000, 14, 5),</v>
       </c>
     </row>
@@ -42757,11 +42766,11 @@
         <v>38</v>
       </c>
       <c r="F46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="H46" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2034/31/12',  10500, 15, 5),</v>
       </c>
     </row>
@@ -42780,11 +42789,11 @@
         <v>38</v>
       </c>
       <c r="F47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="H47" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2035/31/12',  11000, 15, 5),</v>
       </c>
     </row>
@@ -42803,11 +42812,11 @@
         <v>38</v>
       </c>
       <c r="F48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="H48" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2036/31/12',  11500, 15, 5),</v>
       </c>
     </row>
@@ -42826,11 +42835,11 @@
         <v>39</v>
       </c>
       <c r="F49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="H49" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2034/31/12',  10000, 16, 6),</v>
       </c>
     </row>
@@ -42849,11 +42858,11 @@
         <v>39</v>
       </c>
       <c r="F50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="H50" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2035/31/12',  10500, 16, 6),</v>
       </c>
     </row>
@@ -42872,11 +42881,11 @@
         <v>39</v>
       </c>
       <c r="F51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="H51" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2036/31/12',  11000, 16, 6),</v>
       </c>
     </row>
@@ -42895,11 +42904,11 @@
         <v>40</v>
       </c>
       <c r="F52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="H52" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2034/31/12',  10000, 17, 6),</v>
       </c>
     </row>
@@ -42918,11 +42927,11 @@
         <v>40</v>
       </c>
       <c r="F53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="H53" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2035/31/12',  10500, 17, 6),</v>
       </c>
     </row>
@@ -42941,11 +42950,11 @@
         <v>40</v>
       </c>
       <c r="F54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="H54" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2036/31/12',  11000, 17, 6),</v>
       </c>
     </row>
@@ -42964,11 +42973,11 @@
         <v>41</v>
       </c>
       <c r="F55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="H55" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2034/31/12',  12000, 18, 6),</v>
       </c>
     </row>
@@ -42987,11 +42996,11 @@
         <v>41</v>
       </c>
       <c r="F56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="H56" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2035/31/12',  13000, 18, 6),</v>
       </c>
     </row>
@@ -43010,11 +43019,11 @@
         <v>41</v>
       </c>
       <c r="F57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="H57" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2036/31/12',  10000, 18, 6),</v>
       </c>
     </row>
@@ -43033,11 +43042,11 @@
         <v>42</v>
       </c>
       <c r="F58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="H58" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2034/31/12',  10500, 19, 7),</v>
       </c>
     </row>
@@ -43056,11 +43065,11 @@
         <v>42</v>
       </c>
       <c r="F59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="H59" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2035/31/12',  11000, 19, 7),</v>
       </c>
     </row>
@@ -43079,11 +43088,11 @@
         <v>42</v>
       </c>
       <c r="F60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="H60" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2036/31/12',  11500, 19, 7),</v>
       </c>
     </row>
@@ -43102,11 +43111,11 @@
         <v>43</v>
       </c>
       <c r="F61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="H61" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2034/31/12',  10000, 20, 7),</v>
       </c>
     </row>
@@ -43125,11 +43134,11 @@
         <v>43</v>
       </c>
       <c r="F62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="H62" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2035/31/12',  10500, 20, 7),</v>
       </c>
     </row>
@@ -43148,11 +43157,11 @@
         <v>43</v>
       </c>
       <c r="F63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="H63" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2036/31/12',  11000, 20, 7),</v>
       </c>
     </row>
@@ -43171,11 +43180,11 @@
         <v>44</v>
       </c>
       <c r="F64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="H64" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2034/31/12',  10000, 21, 7),</v>
       </c>
     </row>
@@ -43194,11 +43203,11 @@
         <v>44</v>
       </c>
       <c r="F65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="H65" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2035/31/12',  10500, 21, 7),</v>
       </c>
     </row>
@@ -43217,11 +43226,11 @@
         <v>44</v>
       </c>
       <c r="F66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2036/31/12',  11000, 21, 7),</v>
       </c>
     </row>
@@ -43240,11 +43249,11 @@
         <v>45</v>
       </c>
       <c r="F67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>('2034/31/12',  12000, 22, 8),</v>
       </c>
     </row>
@@ -43263,11 +43272,11 @@
         <v>45</v>
       </c>
       <c r="F68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="H68" t="str">
-        <f>CONCATENATE("('", A68,"',  ",B68,", ",C68,", ",F68,"),")</f>
+        <f t="shared" ref="H68:H84" si="5">CONCATENATE("('", A68,"',  ",B68,", ",C68,", ",F68,"),")</f>
         <v>('2035/31/12',  13000, 22, 8),</v>
       </c>
     </row>
@@ -43286,11 +43295,11 @@
         <v>45</v>
       </c>
       <c r="F69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="H69" t="str">
-        <f>CONCATENATE("('", A69,"',  ",B69,", ",C69,", ",F69,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2036/31/12',  10000, 22, 8),</v>
       </c>
     </row>
@@ -43309,11 +43318,11 @@
         <v>46</v>
       </c>
       <c r="F70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="H70" t="str">
-        <f>CONCATENATE("('", A70,"',  ",B70,", ",C70,", ",F70,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2034/31/12',  10500, 23, 8),</v>
       </c>
     </row>
@@ -43332,11 +43341,11 @@
         <v>46</v>
       </c>
       <c r="F71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="H71" t="str">
-        <f>CONCATENATE("('", A71,"',  ",B71,", ",C71,", ",F71,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2035/31/12',  11000, 23, 8),</v>
       </c>
     </row>
@@ -43355,11 +43364,11 @@
         <v>46</v>
       </c>
       <c r="F72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="H72" t="str">
-        <f>CONCATENATE("('", A72,"',  ",B72,", ",C72,", ",F72,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2036/31/12',  11500, 23, 8),</v>
       </c>
     </row>
@@ -43378,11 +43387,11 @@
         <v>47</v>
       </c>
       <c r="F73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="H73" t="str">
-        <f>CONCATENATE("('", A73,"',  ",B73,", ",C73,", ",F73,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2034/31/12',  10000, 24, 8),</v>
       </c>
     </row>
@@ -43394,18 +43403,18 @@
         <v>10500</v>
       </c>
       <c r="C74">
-        <f t="shared" ref="C74:C90" si="4">C71+1</f>
+        <f t="shared" ref="C74:C84" si="6">C71+1</f>
         <v>24</v>
       </c>
       <c r="D74" t="s">
         <v>47</v>
       </c>
       <c r="F74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="H74" t="str">
-        <f>CONCATENATE("('", A74,"',  ",B74,", ",C74,", ",F74,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2035/31/12',  10500, 24, 8),</v>
       </c>
     </row>
@@ -43417,18 +43426,18 @@
         <v>11000</v>
       </c>
       <c r="C75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="D75" t="s">
         <v>47</v>
       </c>
       <c r="F75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="H75" t="str">
-        <f>CONCATENATE("('", A75,"',  ",B75,", ",C75,", ",F75,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2036/31/12',  11000, 24, 8),</v>
       </c>
     </row>
@@ -43440,18 +43449,18 @@
         <v>10000</v>
       </c>
       <c r="C76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="D76" t="s">
         <v>48</v>
       </c>
       <c r="F76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="H76" t="str">
-        <f>CONCATENATE("('", A76,"',  ",B76,", ",C76,", ",F76,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2034/31/12',  10000, 25, 9),</v>
       </c>
     </row>
@@ -43463,18 +43472,18 @@
         <v>10500</v>
       </c>
       <c r="C77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="D77" t="s">
         <v>48</v>
       </c>
       <c r="F77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="H77" t="str">
-        <f>CONCATENATE("('", A77,"',  ",B77,", ",C77,", ",F77,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2035/31/12',  10500, 25, 9),</v>
       </c>
     </row>
@@ -43486,18 +43495,18 @@
         <v>11000</v>
       </c>
       <c r="C78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="D78" t="s">
         <v>48</v>
       </c>
       <c r="F78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="H78" t="str">
-        <f>CONCATENATE("('", A78,"',  ",B78,", ",C78,", ",F78,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2036/31/12',  11000, 25, 9),</v>
       </c>
     </row>
@@ -43509,18 +43518,18 @@
         <v>12000</v>
       </c>
       <c r="C79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
       <c r="D79" t="s">
         <v>49</v>
       </c>
       <c r="F79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="H79" t="str">
-        <f>CONCATENATE("('", A79,"',  ",B79,", ",C79,", ",F79,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2034/31/12',  12000, 26, 9),</v>
       </c>
     </row>
@@ -43532,18 +43541,18 @@
         <v>13000</v>
       </c>
       <c r="C80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
       <c r="D80" t="s">
         <v>49</v>
       </c>
       <c r="F80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="H80" t="str">
-        <f>CONCATENATE("('", A80,"',  ",B80,", ",C80,", ",F80,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2035/31/12',  13000, 26, 9),</v>
       </c>
     </row>
@@ -43555,18 +43564,18 @@
         <v>10000</v>
       </c>
       <c r="C81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
       <c r="D81" t="s">
         <v>49</v>
       </c>
       <c r="F81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="H81" t="str">
-        <f>CONCATENATE("('", A81,"',  ",B81,", ",C81,", ",F81,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2036/31/12',  10000, 26, 9),</v>
       </c>
     </row>
@@ -43578,18 +43587,18 @@
         <v>10500</v>
       </c>
       <c r="C82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="D82" t="s">
         <v>50</v>
       </c>
       <c r="F82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="H82" t="str">
-        <f>CONCATENATE("('", A82,"',  ",B82,", ",C82,", ",F82,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2034/31/12',  10500, 27, 9),</v>
       </c>
     </row>
@@ -43601,18 +43610,18 @@
         <v>11000</v>
       </c>
       <c r="C83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="D83" t="s">
         <v>50</v>
       </c>
       <c r="F83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="H83" t="str">
-        <f>CONCATENATE("('", A83,"',  ",B83,", ",C83,", ",F83,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2035/31/12',  11000, 27, 9),</v>
       </c>
     </row>
@@ -43624,18 +43633,18 @@
         <v>11500</v>
       </c>
       <c r="C84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="D84" t="s">
         <v>50</v>
       </c>
       <c r="F84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="H84" t="str">
-        <f>CONCATENATE("('", A84,"',  ",B84,", ",C84,", ",F84,"),")</f>
+        <f t="shared" si="5"/>
         <v>('2036/31/12',  11500, 27, 9),</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Script crudos con agentes en la misma estacion
</commit_message>
<xml_diff>
--- a/scripts/Script.xlsx
+++ b/scripts/Script.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Lugar" sheetId="1" r:id="rId1"/>
@@ -8872,7 +8872,7 @@
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="166" formatCode="\.\o\rg\.\ve"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -8935,6 +8935,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -8993,7 +9000,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -9032,6 +9039,11 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -10315,18 +10327,18 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="25" t="s">
         <v>2643</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22" t="s">
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25" t="s">
         <v>2644</v>
       </c>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
       <c r="L4" s="12"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -13121,8 +13133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J19" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4:U33"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5:Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13166,16 +13178,16 @@
       <c r="M3" t="s">
         <v>2930</v>
       </c>
-      <c r="N3" s="23" t="s">
+      <c r="N3" s="26" t="s">
         <v>2870</v>
       </c>
-      <c r="O3" s="25"/>
-      <c r="P3" s="23" t="s">
+      <c r="O3" s="28"/>
+      <c r="P3" s="26" t="s">
         <v>2869</v>
       </c>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="25"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="28"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -13559,7 +13571,7 @@
         <v>1</v>
       </c>
       <c r="P9" s="15">
-        <f t="shared" ref="P9:P27" si="5">P7+1</f>
+        <f t="shared" ref="N9:P27" si="5">P7+1</f>
         <v>3</v>
       </c>
       <c r="Q9" s="16">
@@ -13892,14 +13904,12 @@
         <v>9</v>
       </c>
       <c r="N14">
-        <f>N13+1</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O14">
         <v>2</v>
       </c>
       <c r="P14" s="15">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="Q14" s="16">
@@ -13914,7 +13924,7 @@
       </c>
       <c r="U14" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/texto2.txt', 'texto', 'Conflictos entre paises por poder II', 'tecnica', 610, 75, 80 , '2034-05-06 01:00:00', '2035-01-05 01:00:00', 2, 1, null, 6, 2, 5, 2, '2034-01-06 01:00:00', 19),</v>
+        <v>('crudo_contenido/texto2.txt', 'texto', 'Conflictos entre paises por poder II', 'tecnica', 610, 75, 80 , '2034-05-06 01:00:00', '2035-01-05 01:00:00', 2, 1, null, 5, 2, 5, 2, '2034-01-06 01:00:00', 19),</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -14030,12 +14040,10 @@
         <v>9</v>
       </c>
       <c r="N16">
-        <f>N15+1</f>
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="O16">
-        <f>O13+1</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="P16" s="17">
         <v>27</v>
@@ -14051,7 +14059,7 @@
       </c>
       <c r="U16" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/texto2.txt', 'texto', 'Resultados de los conflictos I', 'abierta', 630, 85, 85 , '2034-01-06 01:00:00', '2035-01-06 01:00:00', 2, 8, null, 7, 3, 27, 9, '2034-01-05 01:00:00', 101),</v>
+        <v>('crudo_contenido/texto2.txt', 'texto', 'Resultados de los conflictos I', 'abierta', 630, 85, 85 , '2034-01-06 01:00:00', '2035-01-06 01:00:00', 2, 8, null, 27, 9, 27, 9, '2034-01-05 01:00:00', 101),</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -14096,13 +14104,11 @@
       <c r="M17" t="s">
         <v>9</v>
       </c>
-      <c r="N17">
-        <f>N16+1</f>
-        <v>8</v>
-      </c>
-      <c r="O17">
-        <f>O14+1</f>
-        <v>3</v>
+      <c r="N17" s="15">
+        <v>1</v>
+      </c>
+      <c r="O17" s="16">
+        <v>1</v>
       </c>
       <c r="P17" s="15">
         <v>1</v>
@@ -14118,7 +14124,7 @@
       </c>
       <c r="U17" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/texto.txt', 'texto', 'Resultados de los conflictos II', 'tecnica', 640, 90, 95 , '2034-01-09 01:00:00', '2035-01-05 01:00:00', 2, 8, null, 8, 3, 1, 1, '2034-01-05 01:00:00', 1),</v>
+        <v>('crudo_contenido/texto.txt', 'texto', 'Resultados de los conflictos II', 'tecnica', 640, 90, 95 , '2034-01-09 01:00:00', '2035-01-05 01:00:00', 2, 8, null, 1, 1, 1, 1, '2034-01-05 01:00:00', 1),</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -14163,11 +14169,11 @@
       <c r="M18">
         <v>10</v>
       </c>
-      <c r="N18">
-        <v>5</v>
-      </c>
-      <c r="O18">
-        <v>2</v>
+      <c r="N18" s="15">
+        <v>1</v>
+      </c>
+      <c r="O18" s="16">
+        <v>1</v>
       </c>
       <c r="P18" s="15">
         <v>1</v>
@@ -14184,7 +14190,7 @@
       </c>
       <c r="U18" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/texto.txt', 'texto', 'Resultados de conflictos entre grupo de personas', 'secreta', 650, 70, 60 , '2034-01-20 01:00:00', '2035-01-05 01:00:00', 2, 1, 10, 5, 2, 1, 1, '2034-01-06 01:00:00', 3),</v>
+        <v>('crudo_contenido/texto.txt', 'texto', 'Resultados de conflictos entre grupo de personas', 'secreta', 650, 70, 60 , '2034-01-20 01:00:00', '2035-01-05 01:00:00', 2, 1, 10, 1, 1, 1, 1, '2034-01-06 01:00:00', 3),</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -14229,12 +14235,12 @@
       <c r="M19" t="s">
         <v>9</v>
       </c>
-      <c r="N19">
-        <f>N18+1</f>
-        <v>6</v>
-      </c>
-      <c r="O19">
+      <c r="N19" s="15">
+        <f>N17+1</f>
         <v>2</v>
+      </c>
+      <c r="O19" s="16">
+        <v>1</v>
       </c>
       <c r="P19" s="15">
         <f>P17+1</f>
@@ -14252,7 +14258,7 @@
       </c>
       <c r="U19" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/texto.txt', 'texto', 'Resultados de conflictos entre grupo de personas II', 'abierta', 660, 60, 60 , '2034-02-14 01:00:00', '2035-01-06 01:00:00', 3, 8, null, 6, 2, 2, 1, '2034-01-05 01:00:00', 5),</v>
+        <v>('crudo_contenido/texto.txt', 'texto', 'Resultados de conflictos entre grupo de personas II', 'abierta', 660, 60, 60 , '2034-02-14 01:00:00', '2035-01-06 01:00:00', 3, 8, null, 2, 1, 2, 1, '2034-01-05 01:00:00', 5),</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -14296,12 +14302,12 @@
       <c r="M20" t="s">
         <v>9</v>
       </c>
-      <c r="N20">
-        <f>N19+1</f>
-        <v>7</v>
-      </c>
-      <c r="O20">
-        <v>3</v>
+      <c r="N20" s="15">
+        <f>N18+1</f>
+        <v>2</v>
+      </c>
+      <c r="O20" s="16">
+        <v>1</v>
       </c>
       <c r="P20" s="15">
         <f>P18+1</f>
@@ -14319,7 +14325,7 @@
       </c>
       <c r="U20" t="str">
         <f>CONCATENATE("('",B20,"', '",C20,"', '",D20,"', '",E20,"', ",F20,", ",G20,", ",H20," , '",I20,"', ",J20,", ",K20,", ",L20,", ",M20,", ",N20,", ",O20,", ",P20,", ",Q20,", '",R20,"', ",S20,"),")</f>
-        <v>('crudo_contenido/audio.mp3', 'sonido', 'Agresion de grupo de personas en la via publica', 'tecnica', null, 100, null , '2034-03-19 01:00:00', null, 3, 2, null, 7, 3, 2, 1, '2034-01-06 01:00:00', 7),</v>
+        <v>('crudo_contenido/audio.mp3', 'sonido', 'Agresion de grupo de personas en la via publica', 'tecnica', null, 100, null , '2034-03-19 01:00:00', null, 3, 2, null, 2, 1, 2, 1, '2034-01-06 01:00:00', 7),</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -14364,11 +14370,12 @@
       <c r="M21">
         <v>11</v>
       </c>
-      <c r="N21">
-        <v>6</v>
-      </c>
-      <c r="O21">
-        <v>2</v>
+      <c r="N21" s="15">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="O21" s="16">
+        <v>1</v>
       </c>
       <c r="P21" s="15">
         <f t="shared" si="5"/>
@@ -14386,7 +14393,7 @@
       </c>
       <c r="U21" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/audio.mp3', 'sonido', 'Agresion de grupo de personas en la via publica', 'secreta', 660, 90, 85 , '2034-03-12 01:00:00', '2035-01-06 01:00:00', 2, 2, 11, 6, 2, 3, 1, '2034-01-05 01:00:00', 9),</v>
+        <v>('crudo_contenido/audio.mp3', 'sonido', 'Agresion de grupo de personas en la via publica', 'secreta', 660, 90, 85 , '2034-03-12 01:00:00', '2035-01-06 01:00:00', 2, 2, 11, 3, 1, 3, 1, '2034-01-05 01:00:00', 9),</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -14431,12 +14438,12 @@
       <c r="M22" t="s">
         <v>9</v>
       </c>
-      <c r="N22">
-        <f>N21+1</f>
-        <v>7</v>
-      </c>
-      <c r="O22">
+      <c r="N22" s="15">
+        <f t="shared" si="5"/>
         <v>3</v>
+      </c>
+      <c r="O22" s="16">
+        <v>1</v>
       </c>
       <c r="P22" s="15">
         <f t="shared" si="5"/>
@@ -14454,7 +14461,7 @@
       </c>
       <c r="U22" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/audio.mp3', 'sonido', 'Conflictos en calle con individuos', 'abierta', 670, 30, 30 , '2035-01-06 01:00:00', '2035-01-06 01:00:00', 2, 2, null, 7, 3, 3, 1, '2034-01-06 01:00:00', 11),</v>
+        <v>('crudo_contenido/audio.mp3', 'sonido', 'Conflictos en calle con individuos', 'abierta', 670, 30, 30 , '2035-01-06 01:00:00', '2035-01-06 01:00:00', 2, 2, null, 3, 1, 3, 1, '2034-01-06 01:00:00', 11),</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -14499,12 +14506,12 @@
       <c r="M23" t="s">
         <v>9</v>
       </c>
-      <c r="N23">
-        <f>N22+1</f>
-        <v>8</v>
-      </c>
-      <c r="O23">
-        <v>3</v>
+      <c r="N23" s="15">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="O23" s="16">
+        <v>2</v>
       </c>
       <c r="P23" s="15">
         <f t="shared" si="5"/>
@@ -14522,7 +14529,7 @@
       </c>
       <c r="U23" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/formulas.mp4', 'video', 'Formulas para las empresas', 'tecnica', 680, 40, 35 , '2035-02-14 01:00:00', '2035-01-06 01:00:00', 2, 4, null, 8, 3, 4, 2, '2034-01-05 01:00:00', 13),</v>
+        <v>('crudo_contenido/formulas.mp4', 'video', 'Formulas para las empresas', 'tecnica', 680, 40, 35 , '2035-02-14 01:00:00', '2035-01-06 01:00:00', 2, 4, null, 4, 2, 4, 2, '2034-01-05 01:00:00', 13),</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -14567,10 +14574,11 @@
       <c r="M24">
         <v>12</v>
       </c>
-      <c r="N24">
-        <v>6</v>
-      </c>
-      <c r="O24">
+      <c r="N24" s="15">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="O24" s="16">
         <v>2</v>
       </c>
       <c r="P24" s="15">
@@ -14589,7 +14597,7 @@
       </c>
       <c r="U24" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/imagen3.png', 'imagen', 'Planificacin de marketing', 'secreta', 690, 50, 66 , '2034-03-05 01:00:00', '2035-01-06 01:00:00', 2, 3, 12, 6, 2, 4, 2, '2034-01-06 01:00:00', 15),</v>
+        <v>('crudo_contenido/imagen3.png', 'imagen', 'Planificacin de marketing', 'secreta', 690, 50, 66 , '2034-03-05 01:00:00', '2035-01-06 01:00:00', 2, 3, 12, 4, 2, 4, 2, '2034-01-06 01:00:00', 15),</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -14634,12 +14642,12 @@
       <c r="M25" t="s">
         <v>9</v>
       </c>
-      <c r="N25">
-        <f>N24+1</f>
-        <v>7</v>
-      </c>
-      <c r="O25">
-        <v>3</v>
+      <c r="N25" s="15">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="O25" s="16">
+        <v>2</v>
       </c>
       <c r="P25" s="15">
         <f t="shared" si="5"/>
@@ -14657,7 +14665,7 @@
       </c>
       <c r="U25" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/planos.png', 'imagen', 'Investigacion de planos para construcción', 'abierta', 700, 45, 45 , '2035-01-05 01:00:00', '2035-01-06 01:00:00', 2, 8, null, 7, 3, 5, 2, '2034-01-05 01:00:00', 17),</v>
+        <v>('crudo_contenido/planos.png', 'imagen', 'Investigacion de planos para construcción', 'abierta', 700, 45, 45 , '2035-01-05 01:00:00', '2035-01-06 01:00:00', 2, 8, null, 5, 2, 5, 2, '2034-01-05 01:00:00', 17),</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -14702,12 +14710,12 @@
       <c r="M26" t="s">
         <v>9</v>
       </c>
-      <c r="N26">
-        <f>N25+1</f>
-        <v>8</v>
-      </c>
-      <c r="O26">
-        <v>3</v>
+      <c r="N26" s="15">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="O26" s="16">
+        <v>2</v>
       </c>
       <c r="P26" s="15">
         <f t="shared" si="5"/>
@@ -14725,7 +14733,7 @@
       </c>
       <c r="U26" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/planos.png', 'imagen', 'Planificacion de marketing', 'tecnica', 710, 95, 90 , '2034-12-24 01:00:00', '2035-01-06 01:00:00', 2, 3, null, 8, 3, 5, 2, '2034-01-06 01:00:00', 19),</v>
+        <v>('crudo_contenido/planos.png', 'imagen', 'Planificacion de marketing', 'tecnica', 710, 95, 90 , '2034-12-24 01:00:00', '2035-01-06 01:00:00', 2, 3, null, 5, 2, 5, 2, '2034-01-06 01:00:00', 19),</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -14770,12 +14778,12 @@
       <c r="M27" t="s">
         <v>9</v>
       </c>
-      <c r="N27">
-        <f>N26+1</f>
-        <v>9</v>
-      </c>
-      <c r="O27">
-        <v>3</v>
+      <c r="N27" s="15">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="O27" s="16">
+        <v>2</v>
       </c>
       <c r="P27" s="15">
         <f t="shared" si="5"/>
@@ -14793,7 +14801,7 @@
       </c>
       <c r="U27" t="str">
         <f>CONCATENATE("('",B27,"', '",C27,"', '",D27,"', '",E27,"', ",F27,", ",G27,", ",H27," , '",I27,"', '",J27,"', ",K27,", ",L27,", ",M27,", ",N27,", ",O27,", ",P27,", ",Q27,", '",R27,"', ",S27,"),")</f>
-        <v>('crudo_contenido/imagen3.png', 'imagen', 'Organizacion de marketing', 'abierta', 720, 90, 89 , '2034-11-11 01:00:00', '2035-01-05 01:00:00', 3, 3, null, 9, 3, 6, 2, '2034-01-05 01:00:00', 21),</v>
+        <v>('crudo_contenido/imagen3.png', 'imagen', 'Organizacion de marketing', 'abierta', 720, 90, 89 , '2034-11-11 01:00:00', '2035-01-05 01:00:00', 3, 3, null, 6, 2, 6, 2, '2034-01-05 01:00:00', 21),</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
@@ -14837,12 +14845,11 @@
       <c r="M28" t="s">
         <v>9</v>
       </c>
-      <c r="N28">
-        <f>N27+1</f>
-        <v>10</v>
+      <c r="N28" s="15">
+        <v>1</v>
       </c>
       <c r="O28">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P28" s="15">
         <v>1</v>
@@ -14858,7 +14865,7 @@
       </c>
       <c r="U28" t="str">
         <f>CONCATENATE("('",B28,"', '",C28,"', '",D28,"', '",E28,"', ",F28,", ",G28,", ",H28," , '",I28,"', ",J28,", ",K28,", ",L28,", ",M28,", ",N28,", ",O28,", ",P28,", ",Q28,", '",R28,"', ",S28,"),")</f>
-        <v>('crudo_contenido/planos.png', 'imagen', 'Investigacion de planos para construcción', 'abierta', null, 85, null , '2035-01-30 01:00:00', null, 3, 8, null, 10, 4, 1, 1, '2034-01-05 01:00:00', 1),</v>
+        <v>('crudo_contenido/planos.png', 'imagen', 'Investigacion de planos para construcción', 'abierta', null, 85, null , '2035-01-30 01:00:00', null, 3, 8, null, 1, 1, 1, 1, '2034-01-05 01:00:00', 1),</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
@@ -14903,11 +14910,10 @@
         <v>9</v>
       </c>
       <c r="N29">
-        <f t="shared" ref="N29" si="8">N28+1</f>
-        <v>11</v>
-      </c>
-      <c r="O29">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="O29" s="16">
+        <v>1</v>
       </c>
       <c r="P29">
         <v>3</v>
@@ -14923,7 +14929,7 @@
       </c>
       <c r="U29" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por problemas economicos', 'tecnica', 600, 80, 85 , '2035-02-14 01:00:00', '2036-01-06 01:00:00', 2, 8, null, 11, 4, 3, 1, '2034-01-06 01:00:00', 11),</v>
+        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por problemas economicos', 'tecnica', 600, 80, 85 , '2035-02-14 01:00:00', '2036-01-06 01:00:00', 2, 8, null, 3, 1, 3, 1, '2034-01-06 01:00:00', 11),</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -14967,11 +14973,11 @@
       <c r="M30">
         <v>1</v>
       </c>
-      <c r="N30">
-        <v>7</v>
-      </c>
-      <c r="O30">
-        <v>3</v>
+      <c r="N30" s="15">
+        <v>4</v>
+      </c>
+      <c r="O30" s="16">
+        <v>2</v>
       </c>
       <c r="P30" s="15">
         <v>4</v>
@@ -14983,12 +14989,12 @@
         <v>2865</v>
       </c>
       <c r="S30" s="11">
-        <f t="shared" ref="S30:S32" si="9">S29+2</f>
+        <f t="shared" ref="S30:S32" si="8">S29+2</f>
         <v>13</v>
       </c>
       <c r="U30" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part I', 'secreta', 630, 30, 10 , '2035-01-06 01:00:00', '2036-01-06 01:00:00', 2, 6, 1, 7, 3, 4, 2, '2034-01-05 01:00:00', 13),</v>
+        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part I', 'secreta', 630, 30, 10 , '2035-01-06 01:00:00', '2036-01-06 01:00:00', 2, 6, 1, 4, 2, 4, 2, '2034-01-05 01:00:00', 13),</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -15033,14 +15039,15 @@
         <f>M30+2</f>
         <v>3</v>
       </c>
-      <c r="N31">
-        <v>8</v>
-      </c>
-      <c r="O31">
-        <v>3</v>
+      <c r="N31" s="15">
+        <f t="shared" ref="N31:P32" si="9">N29+1</f>
+        <v>4</v>
+      </c>
+      <c r="O31" s="16">
+        <v>2</v>
       </c>
       <c r="P31" s="15">
-        <f t="shared" ref="P31:P32" si="10">P29+1</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="Q31" s="16">
@@ -15050,12 +15057,12 @@
         <v>2866</v>
       </c>
       <c r="S31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="U31" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part II', 'secreta', 680, 70, 90 , '2035-01-09 01:00:00', '2036-01-05 01:00:00', 2, 3, 3, 8, 3, 4, 2, '2034-01-06 01:00:00', 15),</v>
+        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part II', 'secreta', 680, 70, 90 , '2035-01-09 01:00:00', '2036-01-05 01:00:00', 2, 3, 3, 4, 2, 4, 2, '2034-01-06 01:00:00', 15),</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -15097,17 +15104,18 @@
         <v>8</v>
       </c>
       <c r="M32" s="11">
-        <f t="shared" ref="M32:M33" si="11">M31+2</f>
+        <f t="shared" ref="M32:M33" si="10">M31+2</f>
         <v>5</v>
       </c>
-      <c r="N32">
-        <v>9</v>
-      </c>
-      <c r="O32">
-        <v>3</v>
+      <c r="N32" s="15">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="O32" s="16">
+        <v>2</v>
       </c>
       <c r="P32" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="Q32" s="16">
@@ -15117,12 +15125,12 @@
         <v>2865</v>
       </c>
       <c r="S32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="U32" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part I', 'secreta', 720, 90, 85 , '2035-01-20 01:00:00', '2036-01-06 01:00:00', 2, 8, 5, 9, 3, 5, 2, '2034-01-05 01:00:00', 17),</v>
+        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part I', 'secreta', 720, 90, 85 , '2035-01-20 01:00:00', '2036-01-06 01:00:00', 2, 8, 5, 5, 2, 5, 2, '2034-01-05 01:00:00', 17),</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -15164,14 +15172,14 @@
         <v>6</v>
       </c>
       <c r="M33" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
-      <c r="N33">
-        <v>10</v>
+      <c r="N33" s="15">
+        <v>1</v>
       </c>
       <c r="O33">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P33" s="15">
         <v>1</v>
@@ -15187,7 +15195,7 @@
       </c>
       <c r="U33" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part I', 'secreta', 630, 50, 90 , '2035-01-11 01:00:00', '2036-01-05 01:00:00', 2, 6, 7, 10, 4, 1, 1, '2034-01-05 01:00:00', 1),</v>
+        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part I', 'secreta', 630, 50, 90 , '2035-01-11 01:00:00', '2036-01-05 01:00:00', 2, 6, 7, 1, 1, 1, 1, '2034-01-05 01:00:00', 1),</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -15244,9 +15252,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K68"/>
+  <dimension ref="A2:M68"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K3" sqref="K3:K61"/>
     </sheetView>
   </sheetViews>
@@ -15258,12 +15266,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="25" t="s">
         <v>2911</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -15311,17 +15319,17 @@
         <v>2865</v>
       </c>
       <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4" s="17">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="G4" s="23">
+        <v>3</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="K4" t="str">
         <f>CONCATENATE("('",B4,"', ",C4,", ",D4,", '",E4,"',",F4,",",G4,",",H4,"),")</f>
-        <v>('2034-01-05 01:00:00', 60, 1, '2034-01-05 01:00:00',2,1,1),</v>
+        <v>('2034-01-05 01:00:00', 60, 1, '2034-01-05 01:00:00',10,3,1),</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -15335,24 +15343,24 @@
       <c r="C5">
         <v>85</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="22">
         <v>1</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>2866</v>
+      <c r="E5" s="21" t="s">
+        <v>2865</v>
       </c>
       <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5" s="17">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="G5" s="23">
+        <v>2</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" ref="K5:K61" si="0">CONCATENATE("('",B5,"', ",C5,", ",D5,", '",E5,"',",F5,",",G5,",",H5,"),")</f>
-        <v>('2035-01-06 01:00:00', 85, 1, '2034-01-06 01:00:00',4,1,1),</v>
+        <v>('2035-01-06 01:00:00', 85, 1, '2034-01-05 01:00:00',6,2,1),</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -15369,21 +15377,21 @@
       <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6" s="19" t="s">
-        <v>2865</v>
+      <c r="E6" s="21" t="s">
+        <v>2866</v>
       </c>
       <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6" s="17">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="G6" s="23">
+        <v>3</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 30, 2, '2034-01-05 01:00:00',2,1,1),</v>
+        <v>('2034-01-05 01:00:00', 30, 2, '2034-01-06 01:00:00',12,3,1),</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -15397,7 +15405,7 @@
       <c r="C7">
         <v>30</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="22">
         <v>2</v>
       </c>
       <c r="E7" s="19" t="s">
@@ -15406,7 +15414,7 @@
       <c r="F7">
         <v>6</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="23">
         <v>2</v>
       </c>
       <c r="H7">
@@ -15431,21 +15439,21 @@
       <c r="D8">
         <v>3</v>
       </c>
-      <c r="E8" s="19" t="s">
-        <v>2866</v>
+      <c r="E8" s="21" t="s">
+        <v>2865</v>
       </c>
       <c r="F8">
-        <v>8</v>
-      </c>
-      <c r="G8" s="17">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="G8" s="23">
+        <v>3</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-06 01:00:00', 85, 3, '2034-01-06 01:00:00',8,2,1),</v>
+        <v>('2034-01-06 01:00:00', 85, 3, '2034-01-05 01:00:00',10,3,1),</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -15459,7 +15467,7 @@
       <c r="C9">
         <v>90</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="22">
         <v>3</v>
       </c>
       <c r="E9" s="19" t="s">
@@ -15468,7 +15476,7 @@
       <c r="F9">
         <v>18</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="23">
         <v>5</v>
       </c>
       <c r="H9">
@@ -15499,7 +15507,7 @@
       <c r="F10">
         <v>10</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="23">
         <v>3</v>
       </c>
       <c r="H10">
@@ -15521,24 +15529,24 @@
       <c r="C11">
         <v>60</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="22">
         <v>4</v>
       </c>
-      <c r="E11" s="19" t="s">
-        <v>2866</v>
+      <c r="E11" s="21" t="s">
+        <v>2865</v>
       </c>
       <c r="F11">
-        <v>12</v>
-      </c>
-      <c r="G11" s="17">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="G11" s="23">
+        <v>4</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-06 01:00:00', 60, 4, '2034-01-06 01:00:00',12,3,1),</v>
+        <v>('2035-01-06 01:00:00', 60, 4, '2034-01-05 01:00:00',14,4,2),</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -15561,7 +15569,7 @@
       <c r="F12">
         <v>14</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="23">
         <v>4</v>
       </c>
       <c r="H12">
@@ -15583,7 +15591,7 @@
       <c r="C13">
         <v>70</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="22">
         <v>5</v>
       </c>
       <c r="E13" s="19" t="s">
@@ -15592,7 +15600,7 @@
       <c r="F13">
         <v>2</v>
       </c>
-      <c r="G13" s="17">
+      <c r="G13" s="23">
         <v>1</v>
       </c>
       <c r="H13">
@@ -15623,7 +15631,7 @@
       <c r="F14">
         <v>16</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G14" s="23">
         <v>4</v>
       </c>
       <c r="H14">
@@ -15645,7 +15653,7 @@
       <c r="C15">
         <v>85</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="22">
         <v>6</v>
       </c>
       <c r="E15" s="19" t="s">
@@ -15654,7 +15662,7 @@
       <c r="F15">
         <v>18</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="23">
         <v>5</v>
       </c>
       <c r="H15">
@@ -15685,7 +15693,7 @@
       <c r="F16">
         <v>20</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G16" s="23">
         <v>5</v>
       </c>
       <c r="H16">
@@ -15707,7 +15715,7 @@
       <c r="C17">
         <v>45</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="22">
         <v>7</v>
       </c>
       <c r="E17" s="19" t="s">
@@ -15716,7 +15724,7 @@
       <c r="F17">
         <v>12</v>
       </c>
-      <c r="G17" s="17">
+      <c r="G17" s="23">
         <v>3</v>
       </c>
       <c r="H17">
@@ -15747,7 +15755,7 @@
       <c r="F18">
         <v>102</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="23">
         <v>27</v>
       </c>
       <c r="H18">
@@ -15778,7 +15786,7 @@
       <c r="F19">
         <v>10</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G19" s="23">
         <v>3</v>
       </c>
       <c r="H19">
@@ -15800,7 +15808,7 @@
       <c r="C20">
         <v>85</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="22">
         <v>8</v>
       </c>
       <c r="E20" s="19" t="s">
@@ -15809,7 +15817,7 @@
       <c r="F20">
         <v>6</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="23">
         <v>2</v>
       </c>
       <c r="H20">
@@ -15840,7 +15848,7 @@
       <c r="F21">
         <v>2</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="23">
         <v>1</v>
       </c>
       <c r="H21">
@@ -15862,7 +15870,7 @@
       <c r="C22">
         <v>95</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="22">
         <v>9</v>
       </c>
       <c r="E22" s="19" t="s">
@@ -15871,7 +15879,7 @@
       <c r="F22">
         <v>6</v>
       </c>
-      <c r="G22" s="17">
+      <c r="G22" s="23">
         <v>2</v>
       </c>
       <c r="H22">
@@ -15900,17 +15908,17 @@
         <v>2866</v>
       </c>
       <c r="F23">
-        <v>20</v>
-      </c>
-      <c r="G23" s="17">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="G23" s="23">
+        <v>4</v>
       </c>
       <c r="H23">
         <v>2</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-06 01:00:00', 75, 10, '2034-01-06 01:00:00',20,5,2),</v>
+        <v>('2034-01-06 01:00:00', 75, 10, '2034-01-06 01:00:00',16,4,2),</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -15924,24 +15932,24 @@
       <c r="C24">
         <v>80</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="22">
         <v>10</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="F24">
-        <v>22</v>
-      </c>
-      <c r="G24" s="17">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="G24" s="23">
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-05 01:00:00', 80, 10, '2034-01-05 01:00:00',22,6,2),</v>
+        <v>('2035-01-05 01:00:00', 80, 10, '2034-01-05 01:00:00',2,1,1),</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -15964,7 +15972,7 @@
       <c r="F25">
         <v>26</v>
       </c>
-      <c r="G25" s="17">
+      <c r="G25" s="23">
         <v>7</v>
       </c>
       <c r="H25">
@@ -15986,24 +15994,24 @@
       <c r="C26">
         <v>90</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="22">
         <v>11</v>
       </c>
-      <c r="E26" s="19" t="s">
-        <v>2866</v>
+      <c r="E26" s="21" t="s">
+        <v>2865</v>
       </c>
       <c r="F26">
-        <v>28</v>
-      </c>
-      <c r="G26" s="17">
-        <v>7</v>
+        <v>30</v>
+      </c>
+      <c r="G26" s="23">
+        <v>8</v>
       </c>
       <c r="H26">
         <v>3</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-06 01:00:00', 90, 11, '2034-01-06 01:00:00',28,7,3),</v>
+        <v>('2035-01-06 01:00:00', 90, 11, '2034-01-05 01:00:00',30,8,3),</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -16026,7 +16034,7 @@
       <c r="F27">
         <v>30</v>
       </c>
-      <c r="G27" s="17">
+      <c r="G27" s="23">
         <v>8</v>
       </c>
       <c r="H27">
@@ -16048,24 +16056,24 @@
       <c r="C28">
         <v>85</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="22">
         <v>12</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="F28">
-        <v>32</v>
-      </c>
-      <c r="G28" s="17">
-        <v>8</v>
+        <v>34</v>
+      </c>
+      <c r="G28" s="23">
+        <v>9</v>
       </c>
       <c r="H28">
         <v>3</v>
       </c>
       <c r="K28" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-06 01:00:00', 85, 12, '2034-01-06 01:00:00',32,8,3),</v>
+        <v>('2035-01-06 01:00:00', 85, 12, '2034-01-05 01:00:00',34,9,3),</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -16088,7 +16096,7 @@
       <c r="F29">
         <v>40</v>
       </c>
-      <c r="G29" s="17">
+      <c r="G29" s="23">
         <v>10</v>
       </c>
       <c r="H29">
@@ -16110,7 +16118,7 @@
       <c r="C30">
         <v>85</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="22">
         <v>13</v>
       </c>
       <c r="E30" s="19" t="s">
@@ -16119,7 +16127,7 @@
       <c r="F30">
         <v>42</v>
       </c>
-      <c r="G30" s="17">
+      <c r="G30" s="23">
         <v>11</v>
       </c>
       <c r="H30">
@@ -16150,7 +16158,7 @@
       <c r="F31">
         <v>44</v>
       </c>
-      <c r="G31" s="17">
+      <c r="G31" s="23">
         <v>11</v>
       </c>
       <c r="H31">
@@ -16172,7 +16180,7 @@
       <c r="C32">
         <v>75</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="22">
         <v>14</v>
       </c>
       <c r="E32" s="19" t="s">
@@ -16181,7 +16189,7 @@
       <c r="F32">
         <v>46</v>
       </c>
-      <c r="G32" s="17">
+      <c r="G32" s="23">
         <v>12</v>
       </c>
       <c r="H32">
@@ -16192,7 +16200,7 @@
         <v>('2035-01-05 01:00:00', 75, 14, '2034-01-05 01:00:00',46,12,4),</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -16212,7 +16220,7 @@
       <c r="F33">
         <v>48</v>
       </c>
-      <c r="G33" s="17">
+      <c r="G33" s="23">
         <v>12</v>
       </c>
       <c r="H33">
@@ -16223,7 +16231,7 @@
         <v>('2034-01-06 01:00:00', 90, 15, '2034-01-06 01:00:00',48,12,4),</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -16243,7 +16251,7 @@
       <c r="F34">
         <v>50</v>
       </c>
-      <c r="G34" s="17">
+      <c r="G34" s="23">
         <v>13</v>
       </c>
       <c r="H34">
@@ -16254,7 +16262,7 @@
         <v>('2034-01-05 01:00:00', 90, 15, '2034-01-05 01:00:00',50,13,5),</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -16265,27 +16273,27 @@
       <c r="C35">
         <v>85</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="22">
         <v>15</v>
       </c>
-      <c r="E35" s="19" t="s">
-        <v>2866</v>
+      <c r="E35" s="21" t="s">
+        <v>2865</v>
       </c>
       <c r="F35">
-        <v>52</v>
-      </c>
-      <c r="G35" s="17">
-        <v>13</v>
+        <v>54</v>
+      </c>
+      <c r="G35" s="23">
+        <v>14</v>
       </c>
       <c r="H35">
         <v>5</v>
       </c>
       <c r="K35" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-06 01:00:00', 85, 15, '2034-01-06 01:00:00',52,13,5),</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>('2035-01-06 01:00:00', 85, 15, '2034-01-05 01:00:00',54,14,5),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -16305,7 +16313,7 @@
       <c r="F36">
         <v>40</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="22">
         <v>10</v>
       </c>
       <c r="H36">
@@ -16316,7 +16324,7 @@
         <v>('2034-01-06 01:00:00', 85, 17, '2034-01-06 01:00:00',40,10,4),</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -16327,16 +16335,16 @@
       <c r="C37">
         <v>80</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="22">
         <v>17</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="21" t="s">
         <v>2866</v>
       </c>
       <c r="F37">
         <v>20</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="22">
         <v>5</v>
       </c>
       <c r="H37">
@@ -16347,7 +16355,7 @@
         <v>('2035-01-06 01:00:00', 80, 17, '2034-01-06 01:00:00',20,5,2),</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -16367,7 +16375,7 @@
       <c r="F38">
         <v>2</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="22">
         <v>1</v>
       </c>
       <c r="H38">
@@ -16378,224 +16386,252 @@
         <v>('2034-01-05 01:00:00', 30, 18, '2034-01-05 01:00:00',2,1,1),</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="24">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>2901</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="24">
         <v>100</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="24">
         <v>18</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="13" t="s">
         <v>2866</v>
       </c>
-      <c r="F39">
-        <v>4</v>
-      </c>
-      <c r="G39">
+      <c r="F39" s="24">
+        <v>8</v>
+      </c>
+      <c r="G39" s="22">
+        <v>2</v>
+      </c>
+      <c r="H39" s="24">
         <v>1</v>
       </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-      <c r="K39" t="str">
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-06 01:00:00', 100, 18, '2034-01-06 01:00:00',4,1,1),</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40">
+        <v>('2035-01-06 01:00:00', 100, 18, '2034-01-06 01:00:00',8,2,1),</v>
+      </c>
+      <c r="L39" s="24"/>
+      <c r="M39" s="24"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="24">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="13" t="s">
         <v>2865</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="24">
         <v>40</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="24">
         <v>19</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="13" t="s">
         <v>2865</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="24">
         <v>22</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="22">
         <v>6</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="24">
         <v>2</v>
       </c>
-      <c r="K40" t="str">
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24" t="str">
         <f t="shared" si="0"/>
         <v>('2034-01-05 01:00:00', 40, 19, '2034-01-05 01:00:00',22,6,2),</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="L40" s="24"/>
+      <c r="M40" s="24"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="24">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B41" s="20" t="s">
         <v>2901</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="24">
         <v>40</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="24">
         <v>19</v>
       </c>
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="13" t="s">
         <v>2866</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="24">
         <v>20</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="22">
         <v>5</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="24">
         <v>2</v>
       </c>
-      <c r="K41" t="str">
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24" t="str">
         <f t="shared" si="0"/>
         <v>('2035-01-06 01:00:00', 40, 19, '2034-01-06 01:00:00',20,5,2),</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="24">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="13" t="s">
         <v>2865</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="24">
         <v>70</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="24">
         <v>20</v>
       </c>
-      <c r="E42" s="19" t="s">
+      <c r="E42" s="13" t="s">
         <v>2865</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="24">
         <v>6</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="22">
         <v>2</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="24">
         <v>1</v>
       </c>
-      <c r="K42" t="str">
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+      <c r="K42" s="24" t="str">
         <f t="shared" si="0"/>
         <v>('2034-01-05 01:00:00', 70, 20, '2034-01-05 01:00:00',6,2,1),</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="L42" s="24"/>
+      <c r="M42" s="24"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="24">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B43" s="20" t="s">
         <v>2901</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="24">
         <v>70</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="24">
         <v>20</v>
       </c>
-      <c r="E43" s="19" t="s">
-        <v>2866</v>
-      </c>
-      <c r="F43">
-        <v>8</v>
-      </c>
-      <c r="G43">
+      <c r="E43" s="21" t="s">
+        <v>2865</v>
+      </c>
+      <c r="F43" s="24">
         <v>2</v>
       </c>
-      <c r="H43">
+      <c r="G43" s="22">
         <v>1</v>
       </c>
-      <c r="K43" t="str">
+      <c r="H43" s="24">
+        <v>1</v>
+      </c>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-06 01:00:00', 70, 20, '2034-01-06 01:00:00',8,2,1),</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44">
+        <v>('2035-01-06 01:00:00', 70, 20, '2034-01-05 01:00:00',2,1,1),</v>
+      </c>
+      <c r="L43" s="24"/>
+      <c r="M43" s="24"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="24">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="13" t="s">
         <v>2865</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="24">
         <v>60</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="24">
         <v>21</v>
       </c>
-      <c r="E44" s="19" t="s">
-        <v>2865</v>
-      </c>
-      <c r="F44">
-        <v>10</v>
-      </c>
-      <c r="G44">
-        <v>3</v>
-      </c>
-      <c r="H44">
-        <v>1</v>
-      </c>
-      <c r="K44" t="str">
+      <c r="E44" s="21" t="s">
+        <v>2866</v>
+      </c>
+      <c r="F44" s="24">
+        <v>16</v>
+      </c>
+      <c r="G44" s="22">
+        <v>4</v>
+      </c>
+      <c r="H44" s="24">
+        <v>2</v>
+      </c>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" s="24" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 60, 21, '2034-01-05 01:00:00',10,3,1),</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45">
+        <v>('2034-01-05 01:00:00', 60, 21, '2034-01-06 01:00:00',16,4,2),</v>
+      </c>
+      <c r="L44" s="24"/>
+      <c r="M44" s="24"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="24">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B45" s="20" t="s">
         <v>2901</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="24">
         <v>80</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="24">
         <v>21</v>
       </c>
-      <c r="E45" s="19" t="s">
+      <c r="E45" s="13" t="s">
         <v>2866</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="24">
         <v>12</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="22">
         <v>3</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="24">
         <v>1</v>
       </c>
-      <c r="K45" t="str">
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24" t="str">
         <f t="shared" si="0"/>
         <v>('2035-01-06 01:00:00', 80, 21, '2034-01-06 01:00:00',12,3,1),</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45" s="24"/>
+      <c r="M45" s="24"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -16615,7 +16651,7 @@
       <c r="F46">
         <v>24</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="22">
         <v>6</v>
       </c>
       <c r="H46">
@@ -16626,7 +16662,7 @@
         <v>('2034-01-06 01:00:00', 95, 22, '2034-01-06 01:00:00',24,6,2),</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -16646,7 +16682,7 @@
       <c r="F47">
         <v>40</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="22">
         <v>10</v>
       </c>
       <c r="H47">
@@ -16657,7 +16693,7 @@
         <v>('2035-01-06 01:00:00', 96, 22, '2034-01-06 01:00:00',40,10,4),</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -16677,7 +16713,7 @@
       <c r="F48">
         <v>2</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="22">
         <v>1</v>
       </c>
       <c r="H48">
@@ -16706,17 +16742,17 @@
         <v>2866</v>
       </c>
       <c r="F49">
-        <v>4</v>
-      </c>
-      <c r="G49">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="G49" s="22">
+        <v>5</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K49" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-06 01:00:00', 95, 23, '2034-01-06 01:00:00',4,1,1),</v>
+        <v>('2034-01-06 01:00:00', 95, 23, '2034-01-06 01:00:00',20,5,2),</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -16739,7 +16775,7 @@
       <c r="F50">
         <v>6</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="22">
         <v>2</v>
       </c>
       <c r="H50">
@@ -16770,7 +16806,7 @@
       <c r="F51">
         <v>30</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="22">
         <v>8</v>
       </c>
       <c r="H51">
@@ -16797,7 +16833,7 @@
       <c r="F52">
         <v>2</v>
       </c>
-      <c r="G52" s="17">
+      <c r="G52" s="23">
         <v>1</v>
       </c>
       <c r="H52">
@@ -16818,21 +16854,21 @@
       <c r="D53">
         <v>25</v>
       </c>
-      <c r="E53" s="19" t="s">
-        <v>2866</v>
+      <c r="E53" s="21" t="s">
+        <v>2865</v>
       </c>
       <c r="F53">
+        <v>14</v>
+      </c>
+      <c r="G53" s="23">
         <v>4</v>
       </c>
-      <c r="G53" s="17">
-        <v>1</v>
-      </c>
       <c r="H53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K53" t="str">
         <f t="shared" si="0"/>
-        <v>('2036-01-06 01:00:00', 85, 25, '2034-01-06 01:00:00',4,1,1),</v>
+        <v>('2036-01-06 01:00:00', 85, 25, '2034-01-05 01:00:00',14,4,2),</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -16851,7 +16887,7 @@
       <c r="F54">
         <v>2</v>
       </c>
-      <c r="G54" s="17">
+      <c r="G54" s="23">
         <v>1</v>
       </c>
       <c r="H54">
@@ -16878,7 +16914,7 @@
       <c r="F55">
         <v>6</v>
       </c>
-      <c r="G55" s="17">
+      <c r="G55" s="23">
         <v>2</v>
       </c>
       <c r="H55">
@@ -16905,7 +16941,7 @@
       <c r="F56">
         <v>8</v>
       </c>
-      <c r="G56" s="17">
+      <c r="G56" s="23">
         <v>2</v>
       </c>
       <c r="H56">
@@ -16932,7 +16968,7 @@
       <c r="F57">
         <v>18</v>
       </c>
-      <c r="G57" s="17">
+      <c r="G57" s="23">
         <v>5</v>
       </c>
       <c r="H57">
@@ -16959,7 +16995,7 @@
       <c r="F58">
         <v>10</v>
       </c>
-      <c r="G58" s="17">
+      <c r="G58" s="23">
         <v>3</v>
       </c>
       <c r="H58">
@@ -16981,20 +17017,20 @@
         <v>28</v>
       </c>
       <c r="E59" s="19" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="F59">
-        <v>12</v>
-      </c>
-      <c r="G59" s="17">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="G59" s="23">
+        <v>4</v>
       </c>
       <c r="H59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K59" t="str">
         <f t="shared" si="0"/>
-        <v>('2036-01-06 01:00:00', 60, 28, '2034-01-06 01:00:00',12,3,1),</v>
+        <v>('2036-01-06 01:00:00', 60, 28, '2034-01-05 01:00:00',14,4,2),</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -17013,7 +17049,7 @@
       <c r="F60">
         <v>14</v>
       </c>
-      <c r="G60" s="17">
+      <c r="G60" s="23">
         <v>4</v>
       </c>
       <c r="H60">
@@ -17038,17 +17074,17 @@
         <v>2865</v>
       </c>
       <c r="F61">
-        <v>2</v>
-      </c>
-      <c r="G61" s="17">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="G61" s="23">
+        <v>3</v>
       </c>
       <c r="H61">
         <v>1</v>
       </c>
       <c r="K61" t="str">
         <f t="shared" si="0"/>
-        <v>('2036-01-05 01:00:00', 70, 29, '2034-01-05 01:00:00',2,1,1),</v>
+        <v>('2036-01-05 01:00:00', 70, 29, '2034-01-05 01:00:00',10,3,1),</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -17081,6 +17117,7 @@
     <mergeCell ref="E2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -55538,10 +55575,10 @@
       <c r="C3" t="s">
         <v>2501</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="25" t="s">
         <v>2388</v>
       </c>
-      <c r="F3" s="22"/>
+      <c r="F3" s="25"/>
       <c r="I3" t="s">
         <v>2500</v>
       </c>

</xml_diff>

<commit_message>
SCRIPT DEFINITIVO DE CRUDO_ YA POR FAVOR DIOS O SATAN, EL CRUDO DEBE ESTAR BIEN
</commit_message>
<xml_diff>
--- a/scripts/Script.xlsx
+++ b/scripts/Script.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Lugar" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8914" uniqueCount="2933">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8920" uniqueCount="2931">
   <si>
     <t>id</t>
   </si>
@@ -8749,42 +8749,21 @@
     <t>2034-03-05 01:00:00</t>
   </si>
   <si>
-    <t>2034-05-06 01:00:00</t>
-  </si>
-  <si>
     <t>2034-06-05 01:00:00</t>
   </si>
   <si>
     <t>2034-01-20 01:00:00</t>
   </si>
   <si>
-    <t>2034-02-14 01:00:00</t>
-  </si>
-  <si>
-    <t>2034-03-19 01:00:00</t>
-  </si>
-  <si>
     <t>2034-03-12 01:00:00</t>
   </si>
   <si>
     <t>2035-01-06 01:00:00</t>
   </si>
   <si>
-    <t>2035-02-14 01:00:00</t>
-  </si>
-  <si>
     <t>2035-01-05 01:00:00</t>
   </si>
   <si>
-    <t>2034-12-24 01:00:00</t>
-  </si>
-  <si>
-    <t>2034-11-11 01:00:00</t>
-  </si>
-  <si>
-    <t>2035-01-30 01:00:00</t>
-  </si>
-  <si>
     <t>abierta</t>
   </si>
   <si>
@@ -8845,15 +8824,6 @@
     <t>Empresa en quiebra por malas decisiones del directivo part II</t>
   </si>
   <si>
-    <t>2035-01-09 01:00:00</t>
-  </si>
-  <si>
-    <t>2035-01-20 01:00:00</t>
-  </si>
-  <si>
-    <t>2035-01-11 01:00:00</t>
-  </si>
-  <si>
     <t>INFORMANTE</t>
   </si>
   <si>
@@ -8861,6 +8831,30 @@
   </si>
   <si>
     <t>2036-01-05 01:00:00</t>
+  </si>
+  <si>
+    <t>2034-12-02 17:00:00</t>
+  </si>
+  <si>
+    <t>2034-05-19 07:00:00</t>
+  </si>
+  <si>
+    <t>2034-11-03 07:00:00</t>
+  </si>
+  <si>
+    <t>2034-10-04 02:00:00</t>
+  </si>
+  <si>
+    <t>2034-07-07 05:00:00</t>
+  </si>
+  <si>
+    <t>2034-02-28 07:00:00</t>
+  </si>
+  <si>
+    <t>2035-03-10 06:00:00</t>
+  </si>
+  <si>
+    <t>2034-07-04 02:00:00</t>
   </si>
 </sst>
 </file>
@@ -9000,7 +8994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -9055,6 +9049,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13133,8 +13137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5:Q33"/>
+    <sheetView topLeftCell="K14" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4:U33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13146,7 +13150,7 @@
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
     <col min="8" max="8" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" style="10" customWidth="1"/>
     <col min="13" max="13" width="13" customWidth="1"/>
     <col min="15" max="15" width="14.140625" customWidth="1"/>
     <col min="16" max="16" width="17.5703125" customWidth="1"/>
@@ -13162,7 +13166,7 @@
     </row>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" t="s">
-        <v>2919</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13172,11 +13176,11 @@
       <c r="H3" t="s">
         <v>2386</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="10" t="s">
         <v>2387</v>
       </c>
       <c r="M3" t="s">
-        <v>2930</v>
+        <v>2920</v>
       </c>
       <c r="N3" s="26" t="s">
         <v>2870</v>
@@ -13217,7 +13221,7 @@
       <c r="I4" t="s">
         <v>2374</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="10" t="s">
         <v>2375</v>
       </c>
       <c r="K4" t="s">
@@ -13251,7 +13255,7 @@
         <v>209</v>
       </c>
       <c r="U4" t="s">
-        <v>2919</v>
+        <v>2912</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -13279,11 +13283,11 @@
       <c r="H5">
         <v>85</v>
       </c>
-      <c r="I5" s="13" t="s">
-        <v>2889</v>
-      </c>
-      <c r="J5" s="20" t="s">
-        <v>2901</v>
+      <c r="I5" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>2923</v>
       </c>
       <c r="K5">
         <v>2</v>
@@ -13314,7 +13318,7 @@
       </c>
       <c r="U5" t="str">
         <f>CONCATENATE("('",B5,"', '",C5,"', '",D5,"', '",E5,"', ",F5,", ",G5,", ",H5," , '",I5,"', '",J5,"', ",K5,", ",L5,", ",M5,", ",N5,", ",O5,", ",P5,", ",Q5,", '",R5,"', ",S5,"),")</f>
-        <v>('crudo_contenido/imagen.jpg', 'imagen', 'Problemas politicos en Vitnam I', 'secreta', 500, 85, 85 , '2034-01-08 01:00:00', '2035-01-06 01:00:00', 2, 1, 1, 1, 1, 1, 1, '2034-01-05 01:00:00', 1),</v>
+        <v>('crudo_contenido/imagen.jpg', 'imagen', 'Problemas politicos en Vitnam I', 'secreta', 500, 85, 85 , '2034-01-05 01:00:00', '2034-12-02 17:00:00', 2, 1, 1, 1, 1, 1, 1, '2034-01-05 01:00:00', 1),</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -13338,16 +13342,16 @@
         <v>550</v>
       </c>
       <c r="G6">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="H6">
         <v>10</v>
       </c>
-      <c r="I6" s="13" t="s">
-        <v>2890</v>
-      </c>
-      <c r="J6" s="20" t="s">
-        <v>2903</v>
+      <c r="I6" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J6" s="31" t="s">
+        <v>2925</v>
       </c>
       <c r="K6">
         <v>2</v>
@@ -13380,7 +13384,7 @@
       </c>
       <c r="U6" t="str">
         <f t="shared" ref="U6:U33" si="3">CONCATENATE("('",B6,"', '",C6,"', '",D6,"', '",E6,"', ",F6,", ",G6,", ",H6," , '",I6,"', '",J6,"', ",K6,", ",L6,", ",M6,", ",N6,", ",O6,", ",P6,", ",Q6,", '",R6,"', ",S6,"),")</f>
-        <v>('crudo_contenido/imagen.jpg', 'imagen', 'Problemas politicos en Vitnam II', 'secreta', 550, 30, 10 , '2034-01-09 01:00:00', '2035-01-05 01:00:00', 2, 7, 2, 1, 1, 1, 1, '2034-01-06 01:00:00', 3),</v>
+        <v>('crudo_contenido/imagen.jpg', 'imagen', 'Problemas politicos en Vitnam II', 'secreta', 550, 87, 10 , '2034-01-05 01:00:00', '2034-11-03 07:00:00', 2, 7, 2, 1, 1, 1, 1, '2034-01-06 01:00:00', 3),</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -13401,20 +13405,20 @@
         <v>2627</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:F27" si="4">F6+10</f>
+        <f t="shared" ref="F7:F33" si="4">F6+10</f>
         <v>560</v>
       </c>
       <c r="G7">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H7">
         <v>90</v>
       </c>
-      <c r="I7" s="13" t="s">
-        <v>2889</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>2903</v>
+      <c r="I7" s="19" t="s">
+        <v>2866</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>2926</v>
       </c>
       <c r="K7">
         <v>2</v>
@@ -13449,7 +13453,7 @@
       </c>
       <c r="U7" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/imagen.jpg', 'imagen', 'Consecuencias de problemas politicos por territorio', 'secreta', 560, 85, 90 , '2034-01-08 01:00:00', '2035-01-05 01:00:00', 2, 8, 3, 2, 1, 2, 1, '2034-01-05 01:00:00', 5),</v>
+        <v>('crudo_contenido/imagen.jpg', 'imagen', 'Consecuencias de problemas politicos por territorio', 'secreta', 560, 88, 90 , '2034-01-06 01:00:00', '2034-10-04 02:00:00', 2, 8, 3, 2, 1, 2, 1, '2034-01-05 01:00:00', 5),</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -13474,16 +13478,16 @@
         <v>570</v>
       </c>
       <c r="G8">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="H8">
         <v>85</v>
       </c>
-      <c r="I8" s="13" t="s">
-        <v>2890</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>2901</v>
+      <c r="I8" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J8" s="32" t="s">
+        <v>2898</v>
       </c>
       <c r="K8">
         <v>2</v>
@@ -13517,7 +13521,7 @@
       </c>
       <c r="U8" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/imagen4.jpg', 'imagen', 'Manifestaciones por cambio de leyes', 'secreta', 570, 50, 85 , '2034-01-09 01:00:00', '2035-01-06 01:00:00', 2, 9, 4, 2, 1, 2, 1, '2034-01-06 01:00:00', 7),</v>
+        <v>('crudo_contenido/imagen4.jpg', 'imagen', 'Manifestaciones por cambio de leyes', 'secreta', 570, 85, 85 , '2034-01-05 01:00:00', '2035-01-06 01:00:00', 2, 9, 4, 2, 1, 2, 1, '2034-01-06 01:00:00', 7),</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -13542,16 +13546,16 @@
         <v>580</v>
       </c>
       <c r="G9">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="H9">
         <v>90</v>
       </c>
-      <c r="I9" s="13" t="s">
-        <v>2891</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>2903</v>
+      <c r="I9" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>2899</v>
       </c>
       <c r="K9">
         <v>2</v>
@@ -13586,7 +13590,7 @@
       </c>
       <c r="U9" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/imagen2.jpg', 'imagen', 'Consecuencias de problemas politicos por petroleo en otros territorios', 'secreta', 580, 60, 90 , '2034-01-10 01:00:00', '2035-01-05 01:00:00', 2, 9, 5, 3, 1, 3, 1, '2034-01-05 01:00:00', 9),</v>
+        <v>('crudo_contenido/imagen2.jpg', 'imagen', 'Consecuencias de problemas politicos por petroleo en otros territorios', 'secreta', 580, 93, 90 , '2034-01-05 01:00:00', '2035-01-05 01:00:00', 2, 9, 5, 3, 1, 3, 1, '2034-01-05 01:00:00', 9),</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -13616,11 +13620,11 @@
       <c r="H10">
         <v>60</v>
       </c>
-      <c r="I10" s="13" t="s">
-        <v>2890</v>
-      </c>
-      <c r="J10" s="20" t="s">
-        <v>2903</v>
+      <c r="I10" s="19" t="s">
+        <v>2866</v>
+      </c>
+      <c r="J10" s="31" t="s">
+        <v>2927</v>
       </c>
       <c r="K10">
         <v>2</v>
@@ -13654,7 +13658,7 @@
       </c>
       <c r="U10" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/imagen2.jpg', 'imagen', 'Resultado de guerras entre paises ', 'secreta', 590, 85, 60 , '2034-01-09 01:00:00', '2035-01-05 01:00:00', 2, 8, 6, 3, 1, 3, 1, '2034-01-06 01:00:00', 11),</v>
+        <v>('crudo_contenido/imagen2.jpg', 'imagen', 'Resultado de guerras entre paises ', 'secreta', 590, 85, 60 , '2034-01-06 01:00:00', '2034-07-07 05:00:00', 2, 8, 6, 3, 1, 3, 1, '2034-01-06 01:00:00', 11),</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -13674,20 +13678,21 @@
       <c r="E11" s="9" t="s">
         <v>2627</v>
       </c>
-      <c r="F11" t="s">
-        <v>9</v>
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>600</v>
       </c>
       <c r="G11">
-        <v>35</v>
-      </c>
-      <c r="H11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>2892</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>9</v>
+        <v>90</v>
+      </c>
+      <c r="H11">
+        <v>90</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>2866</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>2925</v>
       </c>
       <c r="K11">
         <v>3</v>
@@ -13721,8 +13726,8 @@
         <v>13</v>
       </c>
       <c r="U11" t="str">
-        <f>CONCATENATE("('",B11,"', '",C11,"', '",D11,"', '",E11,"', ",F11,", ",G11,", ",H11," , '",I11,"', ",J11,", ",K11,", ",L11,", ",M11,", ",N11,", ",O11,", ",P11,", ",Q11,", '",R11,"', ",S11,"),")</f>
-        <v>('crudo_contenido/imagen2.jpg', 'imagen', 'Consecuencias de problemas politicos ', 'secreta', null, 35, null , '2034-01-11 01:00:00', null, 3, 9, 7, 4, 2, 4, 2, '2034-01-05 01:00:00', 13),</v>
+        <f t="shared" si="3"/>
+        <v>('crudo_contenido/imagen2.jpg', 'imagen', 'Consecuencias de problemas politicos ', 'secreta', 600, 90, 90 , '2034-01-06 01:00:00', '2034-11-03 07:00:00', 3, 9, 7, 4, 2, 4, 2, '2034-01-05 01:00:00', 13),</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -13743,8 +13748,8 @@
         <v>2627</v>
       </c>
       <c r="F12">
-        <f>F10</f>
-        <v>590</v>
+        <f t="shared" si="4"/>
+        <v>610</v>
       </c>
       <c r="G12">
         <v>85</v>
@@ -13752,11 +13757,11 @@
       <c r="H12">
         <v>70</v>
       </c>
-      <c r="I12" s="13" t="s">
-        <v>2893</v>
-      </c>
-      <c r="J12" s="20" t="s">
-        <v>2903</v>
+      <c r="I12" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J12" s="31" t="s">
+        <v>2926</v>
       </c>
       <c r="K12">
         <v>3</v>
@@ -13790,7 +13795,7 @@
       </c>
       <c r="U12" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/imagen4.jpg', 'imagen', 'Manifestaciones por digustos de una población por el abuso de poder', 'secreta', 590, 85, 70 , '2034-02-10 01:00:00', '2035-01-05 01:00:00', 3, 9, 8, 4, 2, 4, 2, '2034-01-06 01:00:00', 15),</v>
+        <v>('crudo_contenido/imagen4.jpg', 'imagen', 'Manifestaciones por digustos de una población por el abuso de poder', 'secreta', 610, 85, 70 , '2034-01-05 01:00:00', '2034-10-04 02:00:00', 3, 9, 8, 4, 2, 4, 2, '2034-01-06 01:00:00', 15),</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -13808,23 +13813,23 @@
         <v>2882</v>
       </c>
       <c r="E13" t="s">
-        <v>2907</v>
+        <v>2900</v>
       </c>
       <c r="F13">
         <f t="shared" si="4"/>
-        <v>600</v>
+        <v>620</v>
       </c>
       <c r="G13">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H13">
         <v>90</v>
       </c>
-      <c r="I13" s="13" t="s">
-        <v>2894</v>
-      </c>
-      <c r="J13" s="20" t="s">
-        <v>2903</v>
+      <c r="I13" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J13" s="32" t="s">
+        <v>2899</v>
       </c>
       <c r="K13">
         <v>2</v>
@@ -13858,7 +13863,7 @@
       </c>
       <c r="U13" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/texto2.txt', 'texto', 'Conflictos entre paises por poder II', 'abierta', 600, 90, 90 , '2034-03-05 01:00:00', '2035-01-05 01:00:00', 2, 1, null, 5, 2, 5, 2, '2034-01-05 01:00:00', 17),</v>
+        <v>('crudo_contenido/texto2.txt', 'texto', 'Conflictos entre paises por poder II', 'abierta', 620, 93, 90 , '2034-01-05 01:00:00', '2035-01-05 01:00:00', 2, 1, null, 5, 2, 5, 2, '2034-01-05 01:00:00', 17),</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -13880,19 +13885,19 @@
       </c>
       <c r="F14">
         <f t="shared" si="4"/>
-        <v>610</v>
+        <v>630</v>
       </c>
       <c r="G14">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="H14">
         <v>80</v>
       </c>
-      <c r="I14" s="13" t="s">
-        <v>2895</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>2903</v>
+      <c r="I14" s="19" t="s">
+        <v>2866</v>
+      </c>
+      <c r="J14" s="32" t="s">
+        <v>2899</v>
       </c>
       <c r="K14">
         <v>2</v>
@@ -13924,7 +13929,7 @@
       </c>
       <c r="U14" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/texto2.txt', 'texto', 'Conflictos entre paises por poder II', 'tecnica', 610, 75, 80 , '2034-05-06 01:00:00', '2035-01-05 01:00:00', 2, 1, null, 5, 2, 5, 2, '2034-01-06 01:00:00', 19),</v>
+        <v>('crudo_contenido/texto2.txt', 'texto', 'Conflictos entre paises por poder II', 'tecnica', 630, 88, 80 , '2034-01-06 01:00:00', '2035-01-05 01:00:00', 2, 1, null, 5, 2, 5, 2, '2034-01-06 01:00:00', 19),</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -13946,19 +13951,19 @@
       </c>
       <c r="F15">
         <f t="shared" si="4"/>
-        <v>620</v>
+        <v>640</v>
       </c>
       <c r="G15">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H15">
         <v>80</v>
       </c>
-      <c r="I15" s="13" t="s">
-        <v>2896</v>
-      </c>
-      <c r="J15" s="20" t="s">
-        <v>2901</v>
+      <c r="I15" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>2928</v>
       </c>
       <c r="K15">
         <v>2</v>
@@ -13994,7 +13999,7 @@
       </c>
       <c r="U15" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/texto2.txt', 'texto', 'Tension entre paises y sus consecuencias', 'secreta', 620, 100, 80 , '2034-06-05 01:00:00', '2035-01-06 01:00:00', 2, 1, 9, 6, 2, 6, 2, '2034-01-05 01:00:00', 21),</v>
+        <v>('crudo_contenido/texto2.txt', 'texto', 'Tension entre paises y sus consecuencias', 'secreta', 640, 90, 80 , '2034-01-05 01:00:00', '2034-02-28 07:00:00', 2, 1, 9, 6, 2, 6, 2, '2034-01-05 01:00:00', 21),</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -14012,11 +14017,11 @@
         <v>2880</v>
       </c>
       <c r="E16" t="s">
-        <v>2907</v>
+        <v>2900</v>
       </c>
       <c r="F16">
         <f t="shared" si="4"/>
-        <v>630</v>
+        <v>650</v>
       </c>
       <c r="G16">
         <v>85</v>
@@ -14024,11 +14029,11 @@
       <c r="H16">
         <v>85</v>
       </c>
-      <c r="I16" s="13" t="s">
-        <v>2866</v>
-      </c>
-      <c r="J16" s="20" t="s">
-        <v>2901</v>
+      <c r="I16" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J16" s="32" t="s">
+        <v>2898</v>
       </c>
       <c r="K16">
         <v>2</v>
@@ -14059,7 +14064,7 @@
       </c>
       <c r="U16" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/texto2.txt', 'texto', 'Resultados de los conflictos I', 'abierta', 630, 85, 85 , '2034-01-06 01:00:00', '2035-01-06 01:00:00', 2, 8, null, 27, 9, 27, 9, '2034-01-05 01:00:00', 101),</v>
+        <v>('crudo_contenido/texto2.txt', 'texto', 'Resultados de los conflictos I', 'abierta', 650, 85, 85 , '2034-01-05 01:00:00', '2035-01-06 01:00:00', 2, 8, null, 27, 9, 27, 9, '2034-01-05 01:00:00', 101),</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -14081,19 +14086,19 @@
       </c>
       <c r="F17">
         <f t="shared" si="4"/>
-        <v>640</v>
+        <v>660</v>
       </c>
       <c r="G17">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H17">
         <v>95</v>
       </c>
-      <c r="I17" s="13" t="s">
-        <v>2890</v>
-      </c>
-      <c r="J17" s="20" t="s">
-        <v>2903</v>
+      <c r="I17" s="19" t="s">
+        <v>2866</v>
+      </c>
+      <c r="J17" s="32" t="s">
+        <v>2899</v>
       </c>
       <c r="K17">
         <v>2</v>
@@ -14124,7 +14129,7 @@
       </c>
       <c r="U17" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/texto.txt', 'texto', 'Resultados de los conflictos II', 'tecnica', 640, 90, 95 , '2034-01-09 01:00:00', '2035-01-05 01:00:00', 2, 8, null, 1, 1, 1, 1, '2034-01-05 01:00:00', 1),</v>
+        <v>('crudo_contenido/texto.txt', 'texto', 'Resultados de los conflictos II', 'tecnica', 660, 88, 95 , '2034-01-06 01:00:00', '2035-01-05 01:00:00', 2, 8, null, 1, 1, 1, 1, '2034-01-05 01:00:00', 1),</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -14146,19 +14151,19 @@
       </c>
       <c r="F18">
         <f t="shared" si="4"/>
-        <v>650</v>
+        <v>670</v>
       </c>
       <c r="G18">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="H18">
         <v>60</v>
       </c>
-      <c r="I18" s="13" t="s">
-        <v>2897</v>
-      </c>
-      <c r="J18" s="20" t="s">
-        <v>2903</v>
+      <c r="I18" s="19" t="s">
+        <v>2866</v>
+      </c>
+      <c r="J18" s="32" t="s">
+        <v>2899</v>
       </c>
       <c r="K18">
         <v>2</v>
@@ -14190,7 +14195,7 @@
       </c>
       <c r="U18" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/texto.txt', 'texto', 'Resultados de conflictos entre grupo de personas', 'secreta', 650, 70, 60 , '2034-01-20 01:00:00', '2035-01-05 01:00:00', 2, 1, 10, 1, 1, 1, 1, '2034-01-06 01:00:00', 3),</v>
+        <v>('crudo_contenido/texto.txt', 'texto', 'Resultados de conflictos entre grupo de personas', 'secreta', 670, 94, 60 , '2034-01-06 01:00:00', '2035-01-05 01:00:00', 2, 1, 10, 1, 1, 1, 1, '2034-01-06 01:00:00', 3),</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -14208,23 +14213,23 @@
         <v>2884</v>
       </c>
       <c r="E19" t="s">
-        <v>2907</v>
+        <v>2900</v>
       </c>
       <c r="F19">
         <f t="shared" si="4"/>
-        <v>660</v>
+        <v>680</v>
       </c>
       <c r="G19">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="H19">
         <v>60</v>
       </c>
-      <c r="I19" s="13" t="s">
-        <v>2898</v>
-      </c>
-      <c r="J19" s="20" t="s">
-        <v>2901</v>
+      <c r="I19" s="19" t="s">
+        <v>2866</v>
+      </c>
+      <c r="J19" s="29" t="s">
+        <v>2928</v>
       </c>
       <c r="K19">
         <v>3</v>
@@ -14258,7 +14263,7 @@
       </c>
       <c r="U19" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/texto.txt', 'texto', 'Resultados de conflictos entre grupo de personas II', 'abierta', 660, 60, 60 , '2034-02-14 01:00:00', '2035-01-06 01:00:00', 3, 8, null, 2, 1, 2, 1, '2034-01-05 01:00:00', 5),</v>
+        <v>('crudo_contenido/texto.txt', 'texto', 'Resultados de conflictos entre grupo de personas II', 'abierta', 680, 88, 60 , '2034-01-06 01:00:00', '2034-02-28 07:00:00', 3, 8, null, 2, 1, 2, 1, '2034-01-05 01:00:00', 5),</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -14270,7 +14275,7 @@
         <v>2636</v>
       </c>
       <c r="C20" t="s">
-        <v>2921</v>
+        <v>2914</v>
       </c>
       <c r="D20" t="s">
         <v>2888</v>
@@ -14278,20 +14283,21 @@
       <c r="E20" t="s">
         <v>2632</v>
       </c>
-      <c r="F20" t="s">
-        <v>9</v>
+      <c r="F20">
+        <f t="shared" si="4"/>
+        <v>690</v>
       </c>
       <c r="G20">
-        <v>100</v>
-      </c>
-      <c r="H20" t="s">
-        <v>9</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>2899</v>
-      </c>
-      <c r="J20" s="10" t="s">
-        <v>9</v>
+        <v>90</v>
+      </c>
+      <c r="H20">
+        <v>90</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J20" s="29" t="s">
+        <v>2929</v>
       </c>
       <c r="K20">
         <v>3</v>
@@ -14324,8 +14330,8 @@
         <v>7</v>
       </c>
       <c r="U20" t="str">
-        <f>CONCATENATE("('",B20,"', '",C20,"', '",D20,"', '",E20,"', ",F20,", ",G20,", ",H20," , '",I20,"', ",J20,", ",K20,", ",L20,", ",M20,", ",N20,", ",O20,", ",P20,", ",Q20,", '",R20,"', ",S20,"),")</f>
-        <v>('crudo_contenido/audio.mp3', 'sonido', 'Agresion de grupo de personas en la via publica', 'tecnica', null, 100, null , '2034-03-19 01:00:00', null, 3, 2, null, 2, 1, 2, 1, '2034-01-06 01:00:00', 7),</v>
+        <f t="shared" si="3"/>
+        <v>('crudo_contenido/audio.mp3', 'sonido', 'Agresion de grupo de personas en la via publica', 'tecnica', 690, 90, 90 , '2034-01-05 01:00:00', '2035-03-10 06:00:00', 3, 2, null, 2, 1, 2, 1, '2034-01-06 01:00:00', 7),</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -14337,7 +14343,7 @@
         <v>2636</v>
       </c>
       <c r="C21" t="s">
-        <v>2921</v>
+        <v>2914</v>
       </c>
       <c r="D21" t="s">
         <v>2888</v>
@@ -14346,20 +14352,20 @@
         <v>2627</v>
       </c>
       <c r="F21">
-        <f>F19</f>
-        <v>660</v>
+        <f t="shared" si="4"/>
+        <v>700</v>
       </c>
       <c r="G21">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H21">
         <v>85</v>
       </c>
-      <c r="I21" s="13" t="s">
-        <v>2900</v>
-      </c>
-      <c r="J21" s="20" t="s">
-        <v>2901</v>
+      <c r="I21" s="19" t="s">
+        <v>2866</v>
+      </c>
+      <c r="J21" s="32" t="s">
+        <v>2898</v>
       </c>
       <c r="K21">
         <v>2</v>
@@ -14393,7 +14399,7 @@
       </c>
       <c r="U21" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/audio.mp3', 'sonido', 'Agresion de grupo de personas en la via publica', 'secreta', 660, 90, 85 , '2034-03-12 01:00:00', '2035-01-06 01:00:00', 2, 2, 11, 3, 1, 3, 1, '2034-01-05 01:00:00', 9),</v>
+        <v>('crudo_contenido/audio.mp3', 'sonido', 'Agresion de grupo de personas en la via publica', 'secreta', 700, 87, 85 , '2034-01-06 01:00:00', '2035-01-06 01:00:00', 2, 2, 11, 3, 1, 3, 1, '2034-01-05 01:00:00', 9),</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -14405,29 +14411,29 @@
         <v>2636</v>
       </c>
       <c r="C22" t="s">
-        <v>2921</v>
+        <v>2914</v>
       </c>
       <c r="D22" t="s">
         <v>2633</v>
       </c>
       <c r="E22" t="s">
-        <v>2907</v>
+        <v>2900</v>
       </c>
       <c r="F22">
         <f t="shared" si="4"/>
-        <v>670</v>
+        <v>710</v>
       </c>
       <c r="G22">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="H22">
         <v>30</v>
       </c>
-      <c r="I22" s="13" t="s">
-        <v>2901</v>
-      </c>
-      <c r="J22" s="20" t="s">
-        <v>2901</v>
+      <c r="I22" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J22" s="32" t="s">
+        <v>2898</v>
       </c>
       <c r="K22">
         <v>2</v>
@@ -14461,7 +14467,7 @@
       </c>
       <c r="U22" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/audio.mp3', 'sonido', 'Conflictos en calle con individuos', 'abierta', 670, 30, 30 , '2035-01-06 01:00:00', '2035-01-06 01:00:00', 2, 2, null, 3, 1, 3, 1, '2034-01-06 01:00:00', 11),</v>
+        <v>('crudo_contenido/audio.mp3', 'sonido', 'Conflictos en calle con individuos', 'abierta', 710, 95, 30 , '2034-01-05 01:00:00', '2035-01-06 01:00:00', 2, 2, null, 3, 1, 3, 1, '2034-01-06 01:00:00', 11),</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -14483,19 +14489,19 @@
       </c>
       <c r="F23">
         <f t="shared" si="4"/>
-        <v>680</v>
+        <v>720</v>
       </c>
       <c r="G23">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="H23">
         <v>35</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>2902</v>
-      </c>
-      <c r="J23" s="20" t="s">
-        <v>2901</v>
+        <v>2865</v>
+      </c>
+      <c r="J23" s="32" t="s">
+        <v>2898</v>
       </c>
       <c r="K23">
         <v>2</v>
@@ -14529,7 +14535,7 @@
       </c>
       <c r="U23" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/formulas.mp4', 'video', 'Formulas para las empresas', 'tecnica', 680, 40, 35 , '2035-02-14 01:00:00', '2035-01-06 01:00:00', 2, 4, null, 4, 2, 4, 2, '2034-01-05 01:00:00', 13),</v>
+        <v>('crudo_contenido/formulas.mp4', 'video', 'Formulas para las empresas', 'tecnica', 720, 87, 35 , '2034-01-05 01:00:00', '2035-01-06 01:00:00', 2, 4, null, 4, 2, 4, 2, '2034-01-05 01:00:00', 13),</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -14551,19 +14557,19 @@
       </c>
       <c r="F24">
         <f t="shared" si="4"/>
-        <v>690</v>
+        <v>730</v>
       </c>
       <c r="G24">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="H24">
         <v>66</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>2894</v>
-      </c>
-      <c r="J24" s="20" t="s">
-        <v>2901</v>
+        <v>2865</v>
+      </c>
+      <c r="J24" s="32" t="s">
+        <v>2898</v>
       </c>
       <c r="K24">
         <v>2</v>
@@ -14597,7 +14603,7 @@
       </c>
       <c r="U24" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/imagen3.png', 'imagen', 'Planificacin de marketing', 'secreta', 690, 50, 66 , '2034-03-05 01:00:00', '2035-01-06 01:00:00', 2, 3, 12, 4, 2, 4, 2, '2034-01-06 01:00:00', 15),</v>
+        <v>('crudo_contenido/imagen3.png', 'imagen', 'Planificacin de marketing', 'secreta', 730, 93, 66 , '2034-01-05 01:00:00', '2035-01-06 01:00:00', 2, 3, 12, 4, 2, 4, 2, '2034-01-06 01:00:00', 15),</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -14615,23 +14621,23 @@
         <v>2642</v>
       </c>
       <c r="E25" t="s">
-        <v>2907</v>
+        <v>2900</v>
       </c>
       <c r="F25">
         <f t="shared" si="4"/>
-        <v>700</v>
+        <v>740</v>
       </c>
       <c r="G25">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="H25">
         <v>45</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>2903</v>
-      </c>
-      <c r="J25" s="20" t="s">
-        <v>2901</v>
+        <v>2865</v>
+      </c>
+      <c r="J25" s="31" t="s">
+        <v>2927</v>
       </c>
       <c r="K25">
         <v>2</v>
@@ -14665,7 +14671,7 @@
       </c>
       <c r="U25" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/planos.png', 'imagen', 'Investigacion de planos para construcción', 'abierta', 700, 45, 45 , '2035-01-05 01:00:00', '2035-01-06 01:00:00', 2, 8, null, 5, 2, 5, 2, '2034-01-05 01:00:00', 17),</v>
+        <v>('crudo_contenido/planos.png', 'imagen', 'Investigacion de planos para construcción', 'abierta', 740, 94, 45 , '2034-01-05 01:00:00', '2034-07-07 05:00:00', 2, 8, null, 5, 2, 5, 2, '2034-01-05 01:00:00', 17),</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -14687,19 +14693,19 @@
       </c>
       <c r="F26">
         <f t="shared" si="4"/>
-        <v>710</v>
+        <v>750</v>
       </c>
       <c r="G26">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H26">
         <v>90</v>
       </c>
-      <c r="I26" s="13" t="s">
-        <v>2904</v>
-      </c>
-      <c r="J26" s="20" t="s">
-        <v>2901</v>
+      <c r="I26" s="19" t="s">
+        <v>2866</v>
+      </c>
+      <c r="J26" s="32" t="s">
+        <v>2898</v>
       </c>
       <c r="K26">
         <v>2</v>
@@ -14733,7 +14739,7 @@
       </c>
       <c r="U26" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/planos.png', 'imagen', 'Planificacion de marketing', 'tecnica', 710, 95, 90 , '2034-12-24 01:00:00', '2035-01-06 01:00:00', 2, 3, null, 5, 2, 5, 2, '2034-01-06 01:00:00', 19),</v>
+        <v>('crudo_contenido/planos.png', 'imagen', 'Planificacion de marketing', 'tecnica', 750, 96, 90 , '2034-01-06 01:00:00', '2035-01-06 01:00:00', 2, 3, null, 5, 2, 5, 2, '2034-01-06 01:00:00', 19),</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -14751,23 +14757,23 @@
         <v>2885</v>
       </c>
       <c r="E27" t="s">
-        <v>2907</v>
+        <v>2900</v>
       </c>
       <c r="F27">
         <f t="shared" si="4"/>
-        <v>720</v>
+        <v>760</v>
       </c>
       <c r="G27">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H27">
         <v>89</v>
       </c>
-      <c r="I27" s="13" t="s">
-        <v>2905</v>
-      </c>
-      <c r="J27" s="20" t="s">
-        <v>2903</v>
+      <c r="I27" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J27" s="31" t="s">
+        <v>2930</v>
       </c>
       <c r="K27">
         <v>3</v>
@@ -14800,8 +14806,8 @@
         <v>21</v>
       </c>
       <c r="U27" t="str">
-        <f>CONCATENATE("('",B27,"', '",C27,"', '",D27,"', '",E27,"', ",F27,", ",G27,", ",H27," , '",I27,"', '",J27,"', ",K27,", ",L27,", ",M27,", ",N27,", ",O27,", ",P27,", ",Q27,", '",R27,"', ",S27,"),")</f>
-        <v>('crudo_contenido/imagen3.png', 'imagen', 'Organizacion de marketing', 'abierta', 720, 90, 89 , '2034-11-11 01:00:00', '2035-01-05 01:00:00', 3, 3, null, 6, 2, 6, 2, '2034-01-05 01:00:00', 21),</v>
+        <f t="shared" si="3"/>
+        <v>('crudo_contenido/imagen3.png', 'imagen', 'Organizacion de marketing', 'abierta', 760, 88, 89 , '2034-01-05 01:00:00', '2034-07-04 02:00:00', 3, 3, null, 6, 2, 6, 2, '2034-01-05 01:00:00', 21),</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
@@ -14819,22 +14825,23 @@
         <v>2642</v>
       </c>
       <c r="E28" t="s">
-        <v>2907</v>
-      </c>
-      <c r="F28" t="s">
-        <v>9</v>
+        <v>2900</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="4"/>
+        <v>770</v>
       </c>
       <c r="G28">
-        <v>85</v>
-      </c>
-      <c r="H28" t="s">
-        <v>9</v>
-      </c>
-      <c r="I28" s="13" t="s">
-        <v>2906</v>
-      </c>
-      <c r="J28" s="20" t="s">
-        <v>9</v>
+        <v>88</v>
+      </c>
+      <c r="H28">
+        <v>88</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J28" s="29" t="s">
+        <v>2924</v>
       </c>
       <c r="K28">
         <v>3</v>
@@ -14864,8 +14871,8 @@
         <v>1</v>
       </c>
       <c r="U28" t="str">
-        <f>CONCATENATE("('",B28,"', '",C28,"', '",D28,"', '",E28,"', ",F28,", ",G28,", ",H28," , '",I28,"', ",J28,", ",K28,", ",L28,", ",M28,", ",N28,", ",O28,", ",P28,", ",Q28,", '",R28,"', ",S28,"),")</f>
-        <v>('crudo_contenido/planos.png', 'imagen', 'Investigacion de planos para construcción', 'abierta', null, 85, null , '2035-01-30 01:00:00', null, 3, 8, null, 1, 1, 1, 1, '2034-01-05 01:00:00', 1),</v>
+        <f t="shared" si="3"/>
+        <v>('crudo_contenido/planos.png', 'imagen', 'Investigacion de planos para construcción', 'abierta', 770, 88, 88 , '2034-01-05 01:00:00', '2034-05-19 07:00:00', 3, 8, null, 1, 1, 1, 1, '2034-01-05 01:00:00', 1),</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
@@ -14874,31 +14881,32 @@
         <v>25</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>2924</v>
+        <v>2917</v>
       </c>
       <c r="C29" t="s">
         <v>2628</v>
       </c>
       <c r="D29" t="s">
-        <v>2923</v>
+        <v>2916</v>
       </c>
       <c r="E29" t="s">
         <v>2632</v>
       </c>
       <c r="F29">
-        <v>600</v>
+        <f t="shared" si="4"/>
+        <v>780</v>
       </c>
       <c r="G29">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H29">
         <v>85</v>
       </c>
-      <c r="I29" s="13" t="s">
-        <v>2902</v>
-      </c>
-      <c r="J29" s="20" t="s">
-        <v>2931</v>
+      <c r="I29" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J29" s="32" t="s">
+        <v>2921</v>
       </c>
       <c r="K29">
         <v>2</v>
@@ -14929,7 +14937,7 @@
       </c>
       <c r="U29" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por problemas economicos', 'tecnica', 600, 80, 85 , '2035-02-14 01:00:00', '2036-01-06 01:00:00', 2, 8, null, 3, 1, 3, 1, '2034-01-06 01:00:00', 11),</v>
+        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por problemas economicos', 'tecnica', 780, 90, 85 , '2034-01-05 01:00:00', '2036-01-06 01:00:00', 2, 8, null, 3, 1, 3, 1, '2034-01-06 01:00:00', 11),</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
@@ -14938,31 +14946,32 @@
         <v>26</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>2924</v>
+        <v>2917</v>
       </c>
       <c r="C30" t="s">
         <v>2628</v>
       </c>
       <c r="D30" t="s">
-        <v>2925</v>
+        <v>2918</v>
       </c>
       <c r="E30" t="s">
         <v>2627</v>
       </c>
       <c r="F30">
-        <v>630</v>
+        <f t="shared" si="4"/>
+        <v>790</v>
       </c>
       <c r="G30">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="H30">
         <v>10</v>
       </c>
-      <c r="I30" s="13" t="s">
-        <v>2901</v>
-      </c>
-      <c r="J30" s="20" t="s">
-        <v>2931</v>
+      <c r="I30" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J30" s="32" t="s">
+        <v>2921</v>
       </c>
       <c r="K30">
         <v>2</v>
@@ -14994,7 +15003,7 @@
       </c>
       <c r="U30" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part I', 'secreta', 630, 30, 10 , '2035-01-06 01:00:00', '2036-01-06 01:00:00', 2, 6, 1, 4, 2, 4, 2, '2034-01-05 01:00:00', 13),</v>
+        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part I', 'secreta', 790, 98, 10 , '2034-01-05 01:00:00', '2036-01-06 01:00:00', 2, 6, 1, 4, 2, 4, 2, '2034-01-05 01:00:00', 13),</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -15003,31 +15012,32 @@
         <v>27</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>2924</v>
+        <v>2917</v>
       </c>
       <c r="C31" t="s">
         <v>2628</v>
       </c>
       <c r="D31" t="s">
-        <v>2926</v>
+        <v>2919</v>
       </c>
       <c r="E31" t="s">
         <v>2627</v>
       </c>
       <c r="F31">
-        <v>680</v>
+        <f t="shared" si="4"/>
+        <v>800</v>
       </c>
       <c r="G31">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="H31">
         <v>90</v>
       </c>
-      <c r="I31" s="13" t="s">
-        <v>2927</v>
-      </c>
-      <c r="J31" s="20" t="s">
-        <v>2932</v>
+      <c r="I31" s="19" t="s">
+        <v>2866</v>
+      </c>
+      <c r="J31" s="32" t="s">
+        <v>2922</v>
       </c>
       <c r="K31">
         <v>2</v>
@@ -15062,7 +15072,7 @@
       </c>
       <c r="U31" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part II', 'secreta', 680, 70, 90 , '2035-01-09 01:00:00', '2036-01-05 01:00:00', 2, 3, 3, 4, 2, 4, 2, '2034-01-06 01:00:00', 15),</v>
+        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part II', 'secreta', 800, 88, 90 , '2034-01-06 01:00:00', '2036-01-05 01:00:00', 2, 3, 3, 4, 2, 4, 2, '2034-01-06 01:00:00', 15),</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -15071,31 +15081,32 @@
         <v>28</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>2924</v>
+        <v>2917</v>
       </c>
       <c r="C32" t="s">
         <v>2628</v>
       </c>
       <c r="D32" t="s">
-        <v>2925</v>
+        <v>2918</v>
       </c>
       <c r="E32" t="s">
         <v>2627</v>
       </c>
       <c r="F32">
-        <v>720</v>
+        <f t="shared" si="4"/>
+        <v>810</v>
       </c>
       <c r="G32">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="H32">
         <v>85</v>
       </c>
-      <c r="I32" s="13" t="s">
-        <v>2928</v>
-      </c>
-      <c r="J32" s="20" t="s">
-        <v>2931</v>
+      <c r="I32" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J32" s="32" t="s">
+        <v>2921</v>
       </c>
       <c r="K32">
         <v>2</v>
@@ -15130,7 +15141,7 @@
       </c>
       <c r="U32" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part I', 'secreta', 720, 90, 85 , '2035-01-20 01:00:00', '2036-01-06 01:00:00', 2, 8, 5, 5, 2, 5, 2, '2034-01-05 01:00:00', 17),</v>
+        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part I', 'secreta', 810, 98, 85 , '2034-01-05 01:00:00', '2036-01-06 01:00:00', 2, 8, 5, 5, 2, 5, 2, '2034-01-05 01:00:00', 17),</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -15139,31 +15150,32 @@
         <v>29</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>2924</v>
+        <v>2917</v>
       </c>
       <c r="C33" t="s">
         <v>2628</v>
       </c>
       <c r="D33" t="s">
-        <v>2925</v>
+        <v>2918</v>
       </c>
       <c r="E33" t="s">
         <v>2627</v>
       </c>
       <c r="F33">
-        <v>630</v>
+        <f t="shared" si="4"/>
+        <v>820</v>
       </c>
       <c r="G33">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="H33">
         <v>90</v>
       </c>
-      <c r="I33" s="13" t="s">
-        <v>2929</v>
-      </c>
-      <c r="J33" s="20" t="s">
-        <v>2932</v>
+      <c r="I33" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="J33" s="32" t="s">
+        <v>2922</v>
       </c>
       <c r="K33">
         <v>2</v>
@@ -15195,7 +15207,7 @@
       </c>
       <c r="U33" t="str">
         <f t="shared" si="3"/>
-        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part I', 'secreta', 630, 50, 90 , '2035-01-11 01:00:00', '2036-01-05 01:00:00', 2, 6, 7, 1, 1, 1, 1, '2034-01-05 01:00:00', 1),</v>
+        <v>('crudo_contenido/images.png', 'imagen', 'Empresa en quiebra por malas decisiones del directivo part I', 'secreta', 820, 88, 90 , '2034-01-05 01:00:00', '2036-01-05 01:00:00', 2, 6, 7, 1, 1, 1, 1, '2034-01-05 01:00:00', 1),</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -15204,7 +15216,7 @@
         <v>30</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>2924</v>
+        <v>2917</v>
       </c>
       <c r="M34" s="11"/>
       <c r="Q34" s="16"/>
@@ -15252,10 +15264,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M68"/>
+  <dimension ref="A2:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K61"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:K67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15267,7 +15279,7 @@
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E2" s="25" t="s">
-        <v>2911</v>
+        <v>2904</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
@@ -15278,28 +15290,28 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>2901</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2902</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2903</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>2905</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2906</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2907</v>
+      </c>
+      <c r="H3" t="s">
         <v>2908</v>
       </c>
-      <c r="C3" t="s">
+      <c r="K3" t="s">
         <v>2909</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2910</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>2912</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2913</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2914</v>
-      </c>
-      <c r="H3" t="s">
-        <v>2915</v>
-      </c>
-      <c r="K3" t="s">
-        <v>2916</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -15310,7 +15322,7 @@
         <v>2865</v>
       </c>
       <c r="C4">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -15329,7 +15341,7 @@
       </c>
       <c r="K4" t="str">
         <f>CONCATENATE("('",B4,"', ",C4,", ",D4,", '",E4,"',",F4,",",G4,",",H4,"),")</f>
-        <v>('2034-01-05 01:00:00', 60, 1, '2034-01-05 01:00:00',10,3,1),</v>
+        <v>('2034-01-05 01:00:00', 85, 1, '2034-01-05 01:00:00',10,3,1),</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -15337,8 +15349,8 @@
         <f>A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>2901</v>
+      <c r="B5" s="30" t="s">
+        <v>2923</v>
       </c>
       <c r="C5">
         <v>85</v>
@@ -15359,20 +15371,20 @@
         <v>1</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" ref="K5:K61" si="0">CONCATENATE("('",B5,"', ",C5,", ",D5,", '",E5,"',",F5,",",G5,",",H5,"),")</f>
-        <v>('2035-01-06 01:00:00', 85, 1, '2034-01-05 01:00:00',6,2,1),</v>
+        <f t="shared" ref="K5:K67" si="0">CONCATENATE("('",B5,"', ",C5,", ",D5,", '",E5,"',",F5,",",G5,",",H5,"),")</f>
+        <v>('2034-12-02 17:00:00', 85, 1, '2034-01-05 01:00:00',6,2,1),</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" ref="A6:A51" si="1">A5+1</f>
+        <f t="shared" ref="A6:A67" si="1">A5+1</f>
         <v>3</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="C6">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -15391,7 +15403,7 @@
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 30, 2, '2034-01-06 01:00:00',12,3,1),</v>
+        <v>('2034-01-05 01:00:00', 90, 2, '2034-01-06 01:00:00',12,3,1),</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -15399,11 +15411,11 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>2903</v>
+      <c r="B7" s="31" t="s">
+        <v>2925</v>
       </c>
       <c r="C7">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="D7" s="22">
         <v>2</v>
@@ -15422,7 +15434,7 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-05 01:00:00', 30, 2, '2034-01-05 01:00:00',6,2,1),</v>
+        <v>('2034-11-03 07:00:00', 85, 2, '2034-01-05 01:00:00',6,2,1),</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -15461,8 +15473,8 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>2903</v>
+      <c r="B9" s="31" t="s">
+        <v>2926</v>
       </c>
       <c r="C9">
         <v>90</v>
@@ -15484,7 +15496,7 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-05 01:00:00', 90, 3, '2034-01-05 01:00:00',18,5,2),</v>
+        <v>('2034-10-04 02:00:00', 90, 3, '2034-01-05 01:00:00',18,5,2),</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -15496,7 +15508,7 @@
         <v>2865</v>
       </c>
       <c r="C10">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -15515,7 +15527,7 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 50, 4, '2034-01-05 01:00:00',10,3,1),</v>
+        <v>('2034-01-05 01:00:00', 90, 4, '2034-01-05 01:00:00',10,3,1),</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -15524,10 +15536,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>2901</v>
+        <v>2898</v>
       </c>
       <c r="C11">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D11" s="22">
         <v>4</v>
@@ -15546,7 +15558,7 @@
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-06 01:00:00', 60, 4, '2034-01-05 01:00:00',14,4,2),</v>
+        <v>('2035-01-06 01:00:00', 80, 4, '2034-01-05 01:00:00',14,4,2),</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -15558,7 +15570,7 @@
         <v>2865</v>
       </c>
       <c r="C12">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -15577,7 +15589,7 @@
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 60, 5, '2034-01-05 01:00:00',14,4,2),</v>
+        <v>('2034-01-05 01:00:00', 90, 5, '2034-01-05 01:00:00',14,4,2),</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -15586,10 +15598,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>2903</v>
+        <v>2899</v>
       </c>
       <c r="C13">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="D13" s="22">
         <v>5</v>
@@ -15608,7 +15620,7 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-05 01:00:00', 70, 5, '2034-01-05 01:00:00',2,1,1),</v>
+        <v>('2035-01-05 01:00:00', 95, 5, '2034-01-05 01:00:00',2,1,1),</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -15620,7 +15632,7 @@
         <v>2866</v>
       </c>
       <c r="C14">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -15639,7 +15651,7 @@
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-06 01:00:00', 80, 6, '2034-01-06 01:00:00',16,4,2),</v>
+        <v>('2034-01-06 01:00:00', 85, 6, '2034-01-06 01:00:00',16,4,2),</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -15647,8 +15659,8 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B15" s="20" t="s">
-        <v>2903</v>
+      <c r="B15" s="31" t="s">
+        <v>2927</v>
       </c>
       <c r="C15">
         <v>85</v>
@@ -15670,7 +15682,7 @@
       </c>
       <c r="K15" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-05 01:00:00', 85, 6, '2034-01-05 01:00:00',18,5,2),</v>
+        <v>('2034-07-07 05:00:00', 85, 6, '2034-01-05 01:00:00',18,5,2),</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -15682,7 +15694,7 @@
         <v>2866</v>
       </c>
       <c r="C16">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="D16">
         <v>7</v>
@@ -15701,7 +15713,7 @@
       </c>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-06 01:00:00', 35, 7, '2034-01-06 01:00:00',20,5,2),</v>
+        <v>('2034-01-06 01:00:00', 90, 7, '2034-01-06 01:00:00',20,5,2),</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -15713,7 +15725,7 @@
         <v>2866</v>
       </c>
       <c r="C17">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="D17" s="22">
         <v>7</v>
@@ -15732,7 +15744,7 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-06 01:00:00', 45, 7, '2034-01-06 01:00:00',12,3,1),</v>
+        <v>('2034-01-06 01:00:00', 90, 7, '2034-01-06 01:00:00',12,3,1),</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -15740,30 +15752,30 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="31" t="s">
+        <v>2925</v>
+      </c>
+      <c r="C18">
+        <v>90</v>
+      </c>
+      <c r="D18" s="22">
+        <v>7</v>
+      </c>
+      <c r="E18" s="21" t="s">
         <v>2865</v>
       </c>
-      <c r="C18">
-        <v>85</v>
-      </c>
-      <c r="D18">
-        <v>8</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>2865</v>
-      </c>
       <c r="F18">
-        <v>102</v>
+        <v>26</v>
       </c>
       <c r="G18" s="23">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="H18">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 85, 8, '2034-01-05 01:00:00',102,27,9),</v>
+        <v>('2034-11-03 07:00:00', 90, 7, '2034-01-05 01:00:00',26,7,3),</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -15784,17 +15796,17 @@
         <v>2865</v>
       </c>
       <c r="F19">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="G19" s="23">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 85, 8, '2034-01-05 01:00:00',10,3,1),</v>
+        <v>('2034-01-05 01:00:00', 85, 8, '2034-01-05 01:00:00',102,27,9),</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -15802,30 +15814,30 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B20" s="20" t="s">
-        <v>2903</v>
+      <c r="B20" s="19" t="s">
+        <v>2865</v>
       </c>
       <c r="C20">
         <v>85</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20">
         <v>8</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="F20">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G20" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-05 01:00:00', 85, 8, '2034-01-05 01:00:00',6,2,1),</v>
+        <v>('2034-01-05 01:00:00', 85, 8, '2034-01-05 01:00:00',10,3,1),</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -15833,30 +15845,30 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>2865</v>
+      <c r="B21" s="31" t="s">
+        <v>2926</v>
       </c>
       <c r="C21">
-        <v>90</v>
-      </c>
-      <c r="D21">
-        <v>9</v>
+        <v>85</v>
+      </c>
+      <c r="D21" s="22">
+        <v>8</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21" s="23">
         <v>2</v>
-      </c>
-      <c r="G21" s="23">
-        <v>1</v>
       </c>
       <c r="H21">
         <v>1</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 90, 9, '2034-01-05 01:00:00',2,1,1),</v>
+        <v>('2034-10-04 02:00:00', 85, 8, '2034-01-05 01:00:00',6,2,1),</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -15864,30 +15876,30 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B22" s="20" t="s">
-        <v>2903</v>
+      <c r="B22" s="19" t="s">
+        <v>2865</v>
       </c>
       <c r="C22">
-        <v>95</v>
-      </c>
-      <c r="D22" s="22">
+        <v>90</v>
+      </c>
+      <c r="D22">
         <v>9</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="F22">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G22" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-05 01:00:00', 95, 9, '2034-01-05 01:00:00',6,2,1),</v>
+        <v>('2034-01-05 01:00:00', 90, 9, '2034-01-05 01:00:00',2,1,1),</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -15895,30 +15907,30 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>2866</v>
+      <c r="B23" s="20" t="s">
+        <v>2899</v>
       </c>
       <c r="C23">
-        <v>75</v>
-      </c>
-      <c r="D23">
-        <v>10</v>
+        <v>95</v>
+      </c>
+      <c r="D23" s="22">
+        <v>9</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="F23">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="G23" s="23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-06 01:00:00', 75, 10, '2034-01-06 01:00:00',16,4,2),</v>
+        <v>('2035-01-05 01:00:00', 95, 9, '2034-01-05 01:00:00',6,2,1),</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -15926,30 +15938,30 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="B24" s="20" t="s">
-        <v>2903</v>
+      <c r="B24" s="19" t="s">
+        <v>2866</v>
       </c>
       <c r="C24">
-        <v>80</v>
-      </c>
-      <c r="D24" s="22">
+        <v>95</v>
+      </c>
+      <c r="D24">
         <v>10</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>2865</v>
+        <v>2866</v>
       </c>
       <c r="F24">
+        <v>16</v>
+      </c>
+      <c r="G24" s="23">
+        <v>4</v>
+      </c>
+      <c r="H24">
         <v>2</v>
-      </c>
-      <c r="G24" s="23">
-        <v>1</v>
-      </c>
-      <c r="H24">
-        <v>1</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-05 01:00:00', 80, 10, '2034-01-05 01:00:00',2,1,1),</v>
+        <v>('2034-01-06 01:00:00', 95, 10, '2034-01-06 01:00:00',16,4,2),</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -15957,30 +15969,30 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>2865</v>
+      <c r="B25" s="20" t="s">
+        <v>2899</v>
       </c>
       <c r="C25">
-        <v>90</v>
-      </c>
-      <c r="D25">
-        <v>11</v>
+        <v>80</v>
+      </c>
+      <c r="D25" s="22">
+        <v>10</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="F25">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="G25" s="23">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 90, 11, '2034-01-05 01:00:00',26,7,3),</v>
+        <v>('2035-01-05 01:00:00', 80, 10, '2034-01-05 01:00:00',2,1,1),</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -15988,30 +16000,30 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B26" s="20" t="s">
-        <v>2901</v>
+      <c r="B26" s="19" t="s">
+        <v>2865</v>
       </c>
       <c r="C26">
         <v>90</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26">
         <v>11</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="F26">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G26" s="23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H26">
         <v>3</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-06 01:00:00', 90, 11, '2034-01-05 01:00:00',30,8,3),</v>
+        <v>('2034-01-05 01:00:00', 90, 11, '2034-01-05 01:00:00',26,7,3),</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -16019,16 +16031,16 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>2865</v>
+      <c r="B27" s="29" t="s">
+        <v>2928</v>
       </c>
       <c r="C27">
-        <v>85</v>
-      </c>
-      <c r="D27">
-        <v>12</v>
-      </c>
-      <c r="E27" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="22">
+        <v>11</v>
+      </c>
+      <c r="E27" s="21" t="s">
         <v>2865</v>
       </c>
       <c r="F27">
@@ -16042,7 +16054,7 @@
       </c>
       <c r="K27" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 85, 12, '2034-01-05 01:00:00',30,8,3),</v>
+        <v>('2034-02-28 07:00:00', 90, 11, '2034-01-05 01:00:00',30,8,3),</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -16050,30 +16062,30 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B28" s="20" t="s">
-        <v>2901</v>
+      <c r="B28" s="19" t="s">
+        <v>2865</v>
       </c>
       <c r="C28">
         <v>85</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28">
         <v>12</v>
       </c>
       <c r="E28" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="F28">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G28" s="23">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H28">
         <v>3</v>
       </c>
       <c r="K28" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-06 01:00:00', 85, 12, '2034-01-05 01:00:00',34,9,3),</v>
+        <v>('2034-01-05 01:00:00', 85, 12, '2034-01-05 01:00:00',30,8,3),</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -16081,30 +16093,30 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>2866</v>
+      <c r="B29" s="20" t="s">
+        <v>2898</v>
       </c>
       <c r="C29">
-        <v>90</v>
-      </c>
-      <c r="D29">
-        <v>13</v>
+        <v>85</v>
+      </c>
+      <c r="D29" s="22">
+        <v>12</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="F29">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G29" s="23">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-06 01:00:00', 90, 13, '2034-01-06 01:00:00',40,10,4),</v>
+        <v>('2035-01-06 01:00:00', 85, 12, '2034-01-05 01:00:00',34,9,3),</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -16112,30 +16124,30 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B30" s="20" t="s">
-        <v>2903</v>
+      <c r="B30" s="19" t="s">
+        <v>2866</v>
       </c>
       <c r="C30">
-        <v>85</v>
-      </c>
-      <c r="D30" s="22">
+        <v>90</v>
+      </c>
+      <c r="D30">
         <v>13</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>2865</v>
+        <v>2866</v>
       </c>
       <c r="F30">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G30" s="23">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H30">
         <v>4</v>
       </c>
       <c r="K30" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-05 01:00:00', 85, 13, '2034-01-05 01:00:00',42,11,4),</v>
+        <v>('2034-01-06 01:00:00', 90, 13, '2034-01-06 01:00:00',40,10,4),</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -16143,20 +16155,20 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B31" s="19" t="s">
-        <v>2866</v>
+      <c r="B31" s="20" t="s">
+        <v>2899</v>
       </c>
       <c r="C31">
-        <v>70</v>
-      </c>
-      <c r="D31">
-        <v>14</v>
+        <v>85</v>
+      </c>
+      <c r="D31" s="22">
+        <v>13</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="F31">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G31" s="23">
         <v>11</v>
@@ -16166,7 +16178,7 @@
       </c>
       <c r="K31" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-06 01:00:00', 70, 14, '2034-01-06 01:00:00',44,11,4),</v>
+        <v>('2035-01-05 01:00:00', 85, 13, '2034-01-05 01:00:00',42,11,4),</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -16174,30 +16186,30 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B32" s="20" t="s">
-        <v>2903</v>
+      <c r="B32" s="19" t="s">
+        <v>2866</v>
       </c>
       <c r="C32">
-        <v>75</v>
-      </c>
-      <c r="D32" s="22">
+        <v>90</v>
+      </c>
+      <c r="D32">
         <v>14</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>2865</v>
+        <v>2866</v>
       </c>
       <c r="F32">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G32" s="23">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H32">
         <v>4</v>
       </c>
       <c r="K32" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-05 01:00:00', 75, 14, '2034-01-05 01:00:00',46,12,4),</v>
+        <v>('2034-01-06 01:00:00', 90, 14, '2034-01-06 01:00:00',44,11,4),</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -16205,20 +16217,20 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>2866</v>
+      <c r="B33" s="20" t="s">
+        <v>2899</v>
       </c>
       <c r="C33">
-        <v>90</v>
-      </c>
-      <c r="D33">
-        <v>15</v>
+        <v>97</v>
+      </c>
+      <c r="D33" s="22">
+        <v>14</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="F33">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G33" s="23">
         <v>12</v>
@@ -16228,7 +16240,7 @@
       </c>
       <c r="K33" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-06 01:00:00', 90, 15, '2034-01-06 01:00:00',48,12,4),</v>
+        <v>('2035-01-05 01:00:00', 97, 14, '2034-01-05 01:00:00',46,12,4),</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -16237,7 +16249,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>2865</v>
+        <v>2866</v>
       </c>
       <c r="C34">
         <v>90</v>
@@ -16246,20 +16258,20 @@
         <v>15</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>2865</v>
+        <v>2866</v>
       </c>
       <c r="F34">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G34" s="23">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H34">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K34" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 90, 15, '2034-01-05 01:00:00',50,13,5),</v>
+        <v>('2034-01-06 01:00:00', 90, 15, '2034-01-06 01:00:00',48,12,4),</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -16267,30 +16279,30 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B35" s="20" t="s">
-        <v>2901</v>
+      <c r="B35" s="19" t="s">
+        <v>2865</v>
       </c>
       <c r="C35">
-        <v>85</v>
-      </c>
-      <c r="D35" s="22">
+        <v>90</v>
+      </c>
+      <c r="D35">
         <v>15</v>
       </c>
-      <c r="E35" s="21" t="s">
+      <c r="E35" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="F35">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G35" s="23">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H35">
         <v>5</v>
       </c>
       <c r="K35" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-06 01:00:00', 85, 15, '2034-01-05 01:00:00',54,14,5),</v>
+        <v>('2034-01-05 01:00:00', 90, 15, '2034-01-05 01:00:00',50,13,5),</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -16298,30 +16310,30 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B36" s="19" t="s">
-        <v>2866</v>
+      <c r="B36" s="29" t="s">
+        <v>2928</v>
       </c>
       <c r="C36">
         <v>85</v>
       </c>
-      <c r="D36">
-        <v>17</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>2866</v>
+      <c r="D36" s="22">
+        <v>15</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>2865</v>
       </c>
       <c r="F36">
-        <v>40</v>
-      </c>
-      <c r="G36" s="22">
-        <v>10</v>
+        <v>54</v>
+      </c>
+      <c r="G36" s="23">
+        <v>14</v>
       </c>
       <c r="H36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K36" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-06 01:00:00', 85, 17, '2034-01-06 01:00:00',40,10,4),</v>
+        <v>('2034-02-28 07:00:00', 85, 15, '2034-01-05 01:00:00',54,14,5),</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -16329,30 +16341,30 @@
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="B37" s="20" t="s">
-        <v>2901</v>
+      <c r="B37" s="21" t="s">
+        <v>2865</v>
       </c>
       <c r="C37">
-        <v>80</v>
-      </c>
-      <c r="D37" s="22">
-        <v>17</v>
+        <v>90</v>
+      </c>
+      <c r="D37" s="24">
+        <v>16</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>2866</v>
+        <v>2865</v>
       </c>
       <c r="F37">
-        <v>20</v>
-      </c>
-      <c r="G37" s="22">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="G37" s="23">
+        <v>4</v>
       </c>
       <c r="H37">
         <v>2</v>
       </c>
       <c r="K37" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-06 01:00:00', 80, 17, '2034-01-06 01:00:00',20,5,2),</v>
+        <v>('2034-01-05 01:00:00', 90, 16, '2034-01-05 01:00:00',14,4,2),</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -16360,273 +16372,257 @@
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>2865</v>
+      <c r="B38" s="21" t="s">
+        <v>2899</v>
       </c>
       <c r="C38">
-        <v>30</v>
-      </c>
-      <c r="D38">
-        <v>18</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>2865</v>
+        <v>90</v>
+      </c>
+      <c r="D38" s="24">
+        <v>16</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>2866</v>
       </c>
       <c r="F38">
-        <v>2</v>
-      </c>
-      <c r="G38" s="22">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="G38" s="23">
+        <v>7</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K38" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 30, 18, '2034-01-05 01:00:00',2,1,1),</v>
+        <v>('2035-01-05 01:00:00', 90, 16, '2034-01-06 01:00:00',28,7,3),</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="24">
+      <c r="A39">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="B39" s="20" t="s">
-        <v>2901</v>
-      </c>
-      <c r="C39" s="24">
+      <c r="B39" s="29" t="s">
+        <v>2929</v>
+      </c>
+      <c r="C39">
+        <v>90</v>
+      </c>
+      <c r="D39" s="22">
+        <v>16</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>2865</v>
+      </c>
+      <c r="F39">
+        <v>42</v>
+      </c>
+      <c r="G39" s="23">
+        <v>11</v>
+      </c>
+      <c r="H39">
+        <v>4</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="0"/>
+        <v>('2035-03-10 06:00:00', 90, 16, '2034-01-05 01:00:00',42,11,4),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f>A36+1</f>
+        <v>34</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>2866</v>
+      </c>
+      <c r="C40">
+        <v>85</v>
+      </c>
+      <c r="D40">
+        <v>17</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>2866</v>
+      </c>
+      <c r="F40">
+        <v>40</v>
+      </c>
+      <c r="G40" s="22">
+        <v>10</v>
+      </c>
+      <c r="H40">
+        <v>4</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="0"/>
+        <v>('2034-01-06 01:00:00', 85, 17, '2034-01-06 01:00:00',40,10,4),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>2898</v>
+      </c>
+      <c r="C41">
+        <v>88</v>
+      </c>
+      <c r="D41" s="22">
+        <v>17</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>2866</v>
+      </c>
+      <c r="F41">
+        <v>20</v>
+      </c>
+      <c r="G41" s="22">
+        <v>5</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="K41" t="str">
+        <f t="shared" si="0"/>
+        <v>('2035-01-06 01:00:00', 88, 17, '2034-01-06 01:00:00',20,5,2),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="C42">
+        <v>90</v>
+      </c>
+      <c r="D42">
+        <v>18</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42" s="22">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="K42" t="str">
+        <f t="shared" si="0"/>
+        <v>('2034-01-05 01:00:00', 90, 18, '2034-01-05 01:00:00',2,1,1),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>2898</v>
+      </c>
+      <c r="C43" s="24">
         <v>100</v>
       </c>
-      <c r="D39" s="24">
+      <c r="D43" s="24">
         <v>18</v>
       </c>
-      <c r="E39" s="13" t="s">
+      <c r="E43" s="13" t="s">
         <v>2866</v>
       </c>
-      <c r="F39" s="24">
+      <c r="F43" s="24">
         <v>8</v>
       </c>
-      <c r="G39" s="22">
+      <c r="G43" s="22">
         <v>2</v>
       </c>
-      <c r="H39" s="24">
+      <c r="H43" s="24">
         <v>1</v>
       </c>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="24" t="str">
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" t="str">
         <f t="shared" si="0"/>
         <v>('2035-01-06 01:00:00', 100, 18, '2034-01-06 01:00:00',8,2,1),</v>
       </c>
-      <c r="L39" s="24"/>
-      <c r="M39" s="24"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="24">
-        <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>2865</v>
-      </c>
-      <c r="C40" s="24">
-        <v>40</v>
-      </c>
-      <c r="D40" s="24">
-        <v>19</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>2865</v>
-      </c>
-      <c r="F40" s="24">
-        <v>22</v>
-      </c>
-      <c r="G40" s="22">
-        <v>6</v>
-      </c>
-      <c r="H40" s="24">
-        <v>2</v>
-      </c>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 40, 19, '2034-01-05 01:00:00',22,6,2),</v>
-      </c>
-      <c r="L40" s="24"/>
-      <c r="M40" s="24"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="24">
+      <c r="L43" s="24"/>
+      <c r="M43" s="24"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="B41" s="20" t="s">
-        <v>2901</v>
-      </c>
-      <c r="C41" s="24">
-        <v>40</v>
-      </c>
-      <c r="D41" s="24">
+      <c r="B44" s="13" t="s">
+        <v>2865</v>
+      </c>
+      <c r="C44" s="24">
+        <v>80</v>
+      </c>
+      <c r="D44" s="24">
         <v>19</v>
       </c>
-      <c r="E41" s="13" t="s">
-        <v>2866</v>
-      </c>
-      <c r="F41" s="24">
-        <v>20</v>
-      </c>
-      <c r="G41" s="22">
-        <v>5</v>
-      </c>
-      <c r="H41" s="24">
+      <c r="E44" s="13" t="s">
+        <v>2865</v>
+      </c>
+      <c r="F44" s="24">
+        <v>22</v>
+      </c>
+      <c r="G44" s="22">
+        <v>6</v>
+      </c>
+      <c r="H44" s="24">
         <v>2</v>
       </c>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="24" t="str">
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+      <c r="K44" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-06 01:00:00', 40, 19, '2034-01-06 01:00:00',20,5,2),</v>
-      </c>
-      <c r="L41" s="24"/>
-      <c r="M41" s="24"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="24">
+        <v>('2034-01-05 01:00:00', 80, 19, '2034-01-05 01:00:00',22,6,2),</v>
+      </c>
+      <c r="L44" s="24"/>
+      <c r="M44" s="24"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="B42" s="13" t="s">
-        <v>2865</v>
-      </c>
-      <c r="C42" s="24">
-        <v>70</v>
-      </c>
-      <c r="D42" s="24">
-        <v>20</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>2865</v>
-      </c>
-      <c r="F42" s="24">
-        <v>6</v>
-      </c>
-      <c r="G42" s="22">
-        <v>2</v>
-      </c>
-      <c r="H42" s="24">
-        <v>1</v>
-      </c>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 70, 20, '2034-01-05 01:00:00',6,2,1),</v>
-      </c>
-      <c r="L42" s="24"/>
-      <c r="M42" s="24"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="24">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>2901</v>
-      </c>
-      <c r="C43" s="24">
-        <v>70</v>
-      </c>
-      <c r="D43" s="24">
-        <v>20</v>
-      </c>
-      <c r="E43" s="21" t="s">
-        <v>2865</v>
-      </c>
-      <c r="F43" s="24">
-        <v>2</v>
-      </c>
-      <c r="G43" s="22">
-        <v>1</v>
-      </c>
-      <c r="H43" s="24">
-        <v>1</v>
-      </c>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24"/>
-      <c r="K43" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>('2035-01-06 01:00:00', 70, 20, '2034-01-05 01:00:00',2,1,1),</v>
-      </c>
-      <c r="L43" s="24"/>
-      <c r="M43" s="24"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="24">
-        <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>2865</v>
-      </c>
-      <c r="C44" s="24">
-        <v>60</v>
-      </c>
-      <c r="D44" s="24">
-        <v>21</v>
-      </c>
-      <c r="E44" s="21" t="s">
-        <v>2866</v>
-      </c>
-      <c r="F44" s="24">
-        <v>16</v>
-      </c>
-      <c r="G44" s="22">
-        <v>4</v>
-      </c>
-      <c r="H44" s="24">
-        <v>2</v>
-      </c>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 60, 21, '2034-01-06 01:00:00',16,4,2),</v>
-      </c>
-      <c r="L44" s="24"/>
-      <c r="M44" s="24"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="24">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
       <c r="B45" s="20" t="s">
-        <v>2901</v>
+        <v>2898</v>
       </c>
       <c r="C45" s="24">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="D45" s="24">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E45" s="13" t="s">
         <v>2866</v>
       </c>
       <c r="F45" s="24">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G45" s="22">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H45" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I45" s="24"/>
       <c r="J45" s="24"/>
-      <c r="K45" s="24" t="str">
+      <c r="K45" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-06 01:00:00', 80, 21, '2034-01-06 01:00:00',12,3,1),</v>
+        <v>('2035-01-06 01:00:00', 94, 19, '2034-01-06 01:00:00',20,5,2),</v>
       </c>
       <c r="L45" s="24"/>
       <c r="M45" s="24"/>
@@ -16634,198 +16630,218 @@
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
-      <c r="B46" s="19" t="s">
-        <v>2866</v>
-      </c>
-      <c r="C46">
-        <v>95</v>
-      </c>
-      <c r="D46">
-        <v>22</v>
-      </c>
-      <c r="E46" s="19" t="s">
-        <v>2866</v>
-      </c>
-      <c r="F46">
-        <v>24</v>
+        <v>40</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>2865</v>
+      </c>
+      <c r="C46" s="24">
+        <v>90</v>
+      </c>
+      <c r="D46" s="24">
+        <v>20</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>2865</v>
+      </c>
+      <c r="F46" s="24">
+        <v>6</v>
       </c>
       <c r="G46" s="22">
-        <v>6</v>
-      </c>
-      <c r="H46">
         <v>2</v>
       </c>
+      <c r="H46" s="24">
+        <v>1</v>
+      </c>
+      <c r="I46" s="24"/>
+      <c r="J46" s="24"/>
       <c r="K46" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-06 01:00:00', 95, 22, '2034-01-06 01:00:00',24,6,2),</v>
-      </c>
+        <v>('2034-01-05 01:00:00', 90, 20, '2034-01-05 01:00:00',6,2,1),</v>
+      </c>
+      <c r="L46" s="24"/>
+      <c r="M46" s="24"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>2901</v>
-      </c>
-      <c r="C47">
+        <v>2898</v>
+      </c>
+      <c r="C47" s="24">
         <v>96</v>
       </c>
-      <c r="D47">
-        <v>22</v>
-      </c>
-      <c r="E47" s="19" t="s">
-        <v>2866</v>
-      </c>
-      <c r="F47">
-        <v>40</v>
+      <c r="D47" s="24">
+        <v>20</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>2865</v>
+      </c>
+      <c r="F47" s="24">
+        <v>2</v>
       </c>
       <c r="G47" s="22">
-        <v>10</v>
-      </c>
-      <c r="H47">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H47" s="24">
+        <v>1</v>
+      </c>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24"/>
       <c r="K47" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-06 01:00:00', 96, 22, '2034-01-06 01:00:00',40,10,4),</v>
-      </c>
+        <v>('2035-01-06 01:00:00', 96, 20, '2034-01-05 01:00:00',2,1,1),</v>
+      </c>
+      <c r="L47" s="24"/>
+      <c r="M47" s="24"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="B48" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="13" t="s">
         <v>2865</v>
       </c>
-      <c r="C48">
-        <v>80</v>
-      </c>
-      <c r="D48">
-        <v>23</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>2865</v>
-      </c>
-      <c r="F48">
+      <c r="C48" s="24">
+        <v>90</v>
+      </c>
+      <c r="D48" s="24">
+        <v>21</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>2866</v>
+      </c>
+      <c r="F48" s="24">
+        <v>16</v>
+      </c>
+      <c r="G48" s="22">
+        <v>4</v>
+      </c>
+      <c r="H48" s="24">
         <v>2</v>
       </c>
-      <c r="G48" s="22">
-        <v>1</v>
-      </c>
-      <c r="H48">
-        <v>1</v>
-      </c>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24"/>
       <c r="K48" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 80, 23, '2034-01-05 01:00:00',2,1,1),</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+        <v>('2034-01-05 01:00:00', 90, 21, '2034-01-06 01:00:00',16,4,2),</v>
+      </c>
+      <c r="L48" s="24"/>
+      <c r="M48" s="24"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="1"/>
-        <v>46</v>
-      </c>
-      <c r="B49" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" s="31" t="s">
+        <v>2927</v>
+      </c>
+      <c r="C49" s="24">
+        <v>98</v>
+      </c>
+      <c r="D49" s="24">
+        <v>21</v>
+      </c>
+      <c r="E49" s="13" t="s">
         <v>2866</v>
       </c>
-      <c r="C49">
-        <v>95</v>
-      </c>
-      <c r="D49">
-        <v>23</v>
-      </c>
-      <c r="E49" s="19" t="s">
-        <v>2866</v>
-      </c>
-      <c r="F49">
-        <v>20</v>
+      <c r="F49" s="24">
+        <v>12</v>
       </c>
       <c r="G49" s="22">
-        <v>5</v>
-      </c>
-      <c r="H49">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H49" s="24">
+        <v>1</v>
+      </c>
+      <c r="I49" s="24"/>
+      <c r="J49" s="24"/>
       <c r="K49" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-06 01:00:00', 95, 23, '2034-01-06 01:00:00',20,5,2),</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+        <v>('2034-07-07 05:00:00', 98, 21, '2034-01-06 01:00:00',12,3,1),</v>
+      </c>
+      <c r="L49" s="24"/>
+      <c r="M49" s="24"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="1"/>
-        <v>47</v>
-      </c>
-      <c r="B50" s="20" t="s">
-        <v>2903</v>
+        <v>44</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>2866</v>
       </c>
       <c r="C50">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D50">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>2865</v>
+        <v>2866</v>
       </c>
       <c r="F50">
+        <v>24</v>
+      </c>
+      <c r="G50" s="22">
         <v>6</v>
       </c>
-      <c r="G50" s="22">
+      <c r="H50">
         <v>2</v>
-      </c>
-      <c r="H50">
-        <v>1</v>
       </c>
       <c r="K50" t="str">
         <f t="shared" si="0"/>
-        <v>('2035-01-05 01:00:00', 90, 23, '2034-01-05 01:00:00',6,2,1),</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+        <v>('2034-01-06 01:00:00', 95, 22, '2034-01-06 01:00:00',24,6,2),</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>2865</v>
+        <v>45</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>2898</v>
       </c>
       <c r="C51">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D51">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E51" s="19" t="s">
-        <v>2865</v>
+        <v>2866</v>
       </c>
       <c r="F51">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G51" s="22">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H51">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K51" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 80, 24, '2034-01-05 01:00:00',30,8,3),</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+        <v>('2035-01-06 01:00:00', 96, 22, '2034-01-06 01:00:00',40,10,4),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
       <c r="B52" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="C52">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D52">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E52" s="19" t="s">
         <v>2865</v>
@@ -16833,7 +16849,7 @@
       <c r="F52">
         <v>2</v>
       </c>
-      <c r="G52" s="23">
+      <c r="G52" s="22">
         <v>1</v>
       </c>
       <c r="H52">
@@ -16841,182 +16857,207 @@
       </c>
       <c r="K52" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 60, 25, '2034-01-05 01:00:00',2,1,1),</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="20" t="s">
-        <v>2931</v>
+        <v>('2034-01-05 01:00:00', 80, 23, '2034-01-05 01:00:00',2,1,1),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>2866</v>
       </c>
       <c r="C53">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="D53">
-        <v>25</v>
-      </c>
-      <c r="E53" s="21" t="s">
-        <v>2865</v>
+        <v>23</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>2866</v>
       </c>
       <c r="F53">
-        <v>14</v>
-      </c>
-      <c r="G53" s="23">
-        <v>4</v>
+        <v>20</v>
+      </c>
+      <c r="G53" s="22">
+        <v>5</v>
       </c>
       <c r="H53">
         <v>2</v>
       </c>
       <c r="K53" t="str">
         <f t="shared" si="0"/>
-        <v>('2036-01-06 01:00:00', 85, 25, '2034-01-05 01:00:00',14,4,2),</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="19" t="s">
-        <v>2865</v>
+        <v>('2034-01-06 01:00:00', 95, 23, '2034-01-06 01:00:00',20,5,2),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="B54" s="31" t="s">
+        <v>2930</v>
       </c>
       <c r="C54">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="D54">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E54" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="F54">
+        <v>6</v>
+      </c>
+      <c r="G54" s="22">
         <v>2</v>
-      </c>
-      <c r="G54" s="23">
-        <v>1</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
       <c r="K54" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 30, 26, '2034-01-05 01:00:00',2,1,1),</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B55" s="20" t="s">
-        <v>2931</v>
+        <v>('2034-07-04 02:00:00', 90, 23, '2034-01-05 01:00:00',6,2,1),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f>A54+1</f>
+        <v>49</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>2865</v>
       </c>
       <c r="C55">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D55">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E55" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="F55">
-        <v>6</v>
-      </c>
-      <c r="G55" s="23">
-        <v>2</v>
+        <v>30</v>
+      </c>
+      <c r="G55" s="22">
+        <v>8</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K55" t="str">
         <f t="shared" si="0"/>
-        <v>('2036-01-06 01:00:00', 30, 26, '2034-01-05 01:00:00',6,2,1),</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+        <v>('2034-01-05 01:00:00', 80, 24, '2034-01-05 01:00:00',30,8,3),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" ref="A56:A67" si="2">A55+1</f>
+        <v>50</v>
+      </c>
       <c r="B56" s="19" t="s">
+        <v>2894</v>
+      </c>
+      <c r="C56">
+        <v>90</v>
+      </c>
+      <c r="D56">
+        <v>24</v>
+      </c>
+      <c r="E56" s="21" t="s">
         <v>2866</v>
       </c>
-      <c r="C56">
-        <v>85</v>
-      </c>
-      <c r="D56">
-        <v>27</v>
-      </c>
-      <c r="E56" s="19" t="s">
-        <v>2866</v>
-      </c>
       <c r="F56">
-        <v>8</v>
-      </c>
-      <c r="G56" s="23">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="G56" s="22">
+        <v>3</v>
       </c>
       <c r="H56">
         <v>1</v>
       </c>
       <c r="K56" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-06 01:00:00', 85, 27, '2034-01-06 01:00:00',8,2,1),</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="20" t="s">
-        <v>2932</v>
+        <v>('2034-03-05 01:00:00', 90, 24, '2034-01-06 01:00:00',12,3,1),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="B57" s="29" t="s">
+        <v>2924</v>
       </c>
       <c r="C57">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D57">
-        <v>27</v>
-      </c>
-      <c r="E57" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" s="21" t="s">
         <v>2865</v>
       </c>
       <c r="F57">
-        <v>18</v>
-      </c>
-      <c r="G57" s="23">
-        <v>5</v>
-      </c>
-      <c r="H57">
-        <v>2</v>
+        <v>66</v>
+      </c>
+      <c r="G57" s="22">
+        <v>17</v>
       </c>
       <c r="K57" t="str">
         <f t="shared" si="0"/>
-        <v>('2036-01-05 01:00:00', 90, 27, '2034-01-05 01:00:00',18,5,2),</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+        <v>('2034-05-19 07:00:00', 95, 24, '2034-01-05 01:00:00',66,17,),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
       <c r="B58" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="C58">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="D58">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E58" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="F58">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G58" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H58">
         <v>1</v>
       </c>
       <c r="K58" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 50, 28, '2034-01-05 01:00:00',10,3,1),</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+        <v>('2034-01-05 01:00:00', 95, 25, '2034-01-05 01:00:00',2,1,1),</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
       <c r="B59" s="20" t="s">
-        <v>2931</v>
+        <v>2921</v>
       </c>
       <c r="C59">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="D59">
-        <v>28</v>
-      </c>
-      <c r="E59" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E59" s="21" t="s">
         <v>2865</v>
       </c>
       <c r="F59">
@@ -17030,86 +17071,280 @@
       </c>
       <c r="K59" t="str">
         <f t="shared" si="0"/>
-        <v>('2036-01-06 01:00:00', 60, 28, '2034-01-05 01:00:00',14,4,2),</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+        <v>('2036-01-06 01:00:00', 85, 25, '2034-01-05 01:00:00',14,4,2),</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
       <c r="B60" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="C60">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="D60">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E60" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="F60">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="G60" s="23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K60" t="str">
         <f t="shared" si="0"/>
-        <v>('2034-01-05 01:00:00', 60, 29, '2034-01-05 01:00:00',14,4,2),</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+        <v>('2034-01-05 01:00:00', 97, 26, '2034-01-05 01:00:00',2,1,1),</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
       <c r="B61" s="20" t="s">
-        <v>2932</v>
+        <v>2921</v>
       </c>
       <c r="C61">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="D61">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E61" s="19" t="s">
         <v>2865</v>
       </c>
       <c r="F61">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G61" s="23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H61">
         <v>1</v>
       </c>
       <c r="K61" t="str">
         <f t="shared" si="0"/>
-        <v>('2036-01-05 01:00:00', 70, 29, '2034-01-05 01:00:00',10,3,1),</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B64" s="20" t="s">
-        <v>2931</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+        <v>('2036-01-06 01:00:00', 98, 26, '2034-01-05 01:00:00',6,2,1),</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="B62" s="19" t="s">
+        <v>2866</v>
+      </c>
+      <c r="C62">
+        <v>85</v>
+      </c>
+      <c r="D62">
+        <v>27</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>2866</v>
+      </c>
+      <c r="F62">
+        <v>8</v>
+      </c>
+      <c r="G62" s="23">
+        <v>2</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="K62" t="str">
+        <f t="shared" si="0"/>
+        <v>('2034-01-06 01:00:00', 85, 27, '2034-01-06 01:00:00',8,2,1),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="B63" s="20" t="s">
+        <v>2922</v>
+      </c>
+      <c r="C63">
+        <v>90</v>
+      </c>
+      <c r="D63">
+        <v>27</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="F63">
+        <v>18</v>
+      </c>
+      <c r="G63" s="23">
+        <v>5</v>
+      </c>
+      <c r="H63">
+        <v>2</v>
+      </c>
+      <c r="K63" t="str">
+        <f t="shared" si="0"/>
+        <v>('2036-01-05 01:00:00', 90, 27, '2034-01-05 01:00:00',18,5,2),</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="B64" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="C64">
+        <v>97</v>
+      </c>
+      <c r="D64">
+        <v>28</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="F64">
+        <v>10</v>
+      </c>
+      <c r="G64" s="23">
+        <v>3</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="K64" t="str">
+        <f t="shared" si="0"/>
+        <v>('2034-01-05 01:00:00', 97, 28, '2034-01-05 01:00:00',10,3,1),</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
       <c r="B65" s="20" t="s">
-        <v>2931</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="20" t="s">
-        <v>2932</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+        <v>2921</v>
+      </c>
+      <c r="C65">
+        <v>98</v>
+      </c>
+      <c r="D65">
+        <v>28</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="F65">
+        <v>14</v>
+      </c>
+      <c r="G65" s="23">
+        <v>4</v>
+      </c>
+      <c r="H65">
+        <v>2</v>
+      </c>
+      <c r="K65" t="str">
+        <f t="shared" si="0"/>
+        <v>('2036-01-06 01:00:00', 98, 28, '2034-01-05 01:00:00',14,4,2),</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="B66" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="C66">
+        <v>89</v>
+      </c>
+      <c r="D66">
+        <v>29</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="F66">
+        <v>14</v>
+      </c>
+      <c r="G66" s="23">
+        <v>4</v>
+      </c>
+      <c r="H66">
+        <v>2</v>
+      </c>
+      <c r="K66" t="str">
+        <f t="shared" si="0"/>
+        <v>('2034-01-05 01:00:00', 89, 29, '2034-01-05 01:00:00',14,4,2),</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="2"/>
+        <v>61</v>
+      </c>
       <c r="B67" s="20" t="s">
-        <v>2931</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="20" t="s">
-        <v>2932</v>
+        <v>2922</v>
+      </c>
+      <c r="C67">
+        <v>87</v>
+      </c>
+      <c r="D67">
+        <v>29</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>2865</v>
+      </c>
+      <c r="F67">
+        <v>10</v>
+      </c>
+      <c r="G67" s="23">
+        <v>3</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="K67" t="str">
+        <f t="shared" si="0"/>
+        <v>('2036-01-05 01:00:00', 87, 29, '2034-01-05 01:00:00',10,3,1),</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B70" s="20" t="s">
+        <v>2921</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B71" s="20" t="s">
+        <v>2921</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B72" s="20" t="s">
+        <v>2922</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B73" s="20" t="s">
+        <v>2921</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B74" s="20" t="s">
+        <v>2922</v>
       </c>
     </row>
   </sheetData>
@@ -17140,19 +17375,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>2908</v>
+        <v>2901</v>
       </c>
       <c r="C3" t="s">
-        <v>2917</v>
+        <v>2910</v>
       </c>
       <c r="D3" t="s">
-        <v>2910</v>
+        <v>2903</v>
       </c>
       <c r="E3" t="s">
-        <v>2918</v>
+        <v>2911</v>
       </c>
       <c r="I3" t="s">
-        <v>2922</v>
+        <v>2915</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -17380,7 +17615,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="C12">
         <v>320</v>
@@ -17405,7 +17640,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="C13">
         <v>335</v>
@@ -17430,7 +17665,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>2900</v>
+        <v>2897</v>
       </c>
       <c r="C14">
         <v>350</v>
@@ -17492,7 +17727,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>2920</v>
+        <v>2913</v>
       </c>
     </row>
   </sheetData>

</xml_diff>